<commit_message>
changed utility slots from 5*2^size to 8*2^size
</commit_message>
<xml_diff>
--- a/Stellaris Rebalance.xlsx
+++ b/Stellaris Rebalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="weapon_components" sheetId="4" r:id="rId1"/>
@@ -21047,10 +21047,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1"/>
+  <dimension ref="B1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21060,9 +21060,15 @@
     <col min="4" max="4" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f>64/3</f>
+        <v>21.333333333333332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weapons rebalanced to cost 25% of utility space to power at equal tiers of weapons and generators
</commit_message>
<xml_diff>
--- a/Stellaris Rebalance.xlsx
+++ b/Stellaris Rebalance.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="737" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="weapon_components" sheetId="4" r:id="rId1"/>
     <sheet name="Weapon Formulas" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Ship Design Balancing" sheetId="5" r:id="rId3"/>
     <sheet name="gen_weapon_components" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="261">
   <si>
     <t># Lines starting with ”#” will be treated as comments.</t>
   </si>
@@ -776,6 +776,36 @@
   <si>
     <t>Corvettes</t>
   </si>
+  <si>
+    <t>Destroyer</t>
+  </si>
+  <si>
+    <t>Cruiser</t>
+  </si>
+  <si>
+    <t>Battleship</t>
+  </si>
+  <si>
+    <t>Should be 24</t>
+  </si>
+  <si>
+    <t>Weapon Slots</t>
+  </si>
+  <si>
+    <t>Utility Slots</t>
+  </si>
+  <si>
+    <t>Weapon Power Size Cost</t>
+  </si>
+  <si>
+    <t>Power/Size</t>
+  </si>
+  <si>
+    <t>Weapon Power/ Size</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
 </sst>
 </file>
 
@@ -861,7 +891,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -884,6 +914,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1304,6 +1335,279 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="105"/>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-6.6666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-6.6666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-426.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-426.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-426.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-3.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-6.6666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-6.6666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-426.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-3.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-6.6666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-6.6666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-213.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-106.66666666666666</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -11908,8 +12212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP121"/>
   <sheetViews>
-    <sheetView topLeftCell="H100" workbookViewId="0">
-      <selection activeCell="O119" sqref="O119"/>
+    <sheetView topLeftCell="L94" workbookViewId="0">
+      <selection activeCell="W104" sqref="W104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12298,11 +12602,11 @@
       <c r="F8" s="12">
         <v>0.2</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="W8">
@@ -12420,7 +12724,9 @@
       <c r="T10" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="U10" s="2"/>
+      <c r="U10" s="13" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
@@ -12494,7 +12800,10 @@
       <c r="T11" s="2">
         <v>0</v>
       </c>
-      <c r="U11" s="2"/>
+      <c r="U11" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C11)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D11+2)*(1+'Weapon Formulas'!B11))</f>
+        <v>-3.333333333333333</v>
+      </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
@@ -12568,7 +12877,10 @@
       <c r="T12" s="2">
         <v>0</v>
       </c>
-      <c r="U12" s="2"/>
+      <c r="U12" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C12)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D12+2)*(1+'Weapon Formulas'!B12))</f>
+        <v>-6.6666666666666661</v>
+      </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
@@ -12642,7 +12954,10 @@
       <c r="T13" s="2">
         <v>0</v>
       </c>
-      <c r="U13" s="2"/>
+      <c r="U13" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C13)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D13+2)*(1+'Weapon Formulas'!B13))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
@@ -12716,7 +13031,10 @@
       <c r="T14" s="2">
         <v>0</v>
       </c>
-      <c r="U14" s="2"/>
+      <c r="U14" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C14)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D14+2)*(1+'Weapon Formulas'!B14))</f>
+        <v>-6.6666666666666661</v>
+      </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
@@ -12790,7 +13108,10 @@
       <c r="T15" s="2">
         <v>0</v>
       </c>
-      <c r="U15" s="2"/>
+      <c r="U15" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C15)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D15+2)*(1+'Weapon Formulas'!B15))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
@@ -12864,7 +13185,10 @@
       <c r="T16" s="2">
         <v>0</v>
       </c>
-      <c r="U16" s="2"/>
+      <c r="U16" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C16)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D16+2)*(1+'Weapon Formulas'!B16))</f>
+        <v>-26.666666666666664</v>
+      </c>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
@@ -12938,7 +13262,10 @@
       <c r="T17" s="2">
         <v>0</v>
       </c>
-      <c r="U17" s="2"/>
+      <c r="U17" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C17)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D17+2)*(1+'Weapon Formulas'!B17))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
@@ -13012,7 +13339,10 @@
       <c r="T18" s="2">
         <v>0</v>
       </c>
-      <c r="U18" s="2"/>
+      <c r="U18" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C18)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D18+2)*(1+'Weapon Formulas'!B18))</f>
+        <v>-26.666666666666664</v>
+      </c>
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
@@ -13086,7 +13416,10 @@
       <c r="T19" s="2">
         <v>0</v>
       </c>
-      <c r="U19" s="2"/>
+      <c r="U19" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C19)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D19+2)*(1+'Weapon Formulas'!B19))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
@@ -13160,7 +13493,10 @@
       <c r="T20" s="2">
         <v>0</v>
       </c>
-      <c r="U20" s="2"/>
+      <c r="U20" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C20)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D20+2)*(1+'Weapon Formulas'!B20))</f>
+        <v>-26.666666666666664</v>
+      </c>
       <c r="X20" s="14"/>
       <c r="Y20" s="14"/>
     </row>
@@ -13236,7 +13572,10 @@
       <c r="T21" s="2">
         <v>0</v>
       </c>
-      <c r="U21" s="2"/>
+      <c r="U21" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C21)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D21+2)*(1+'Weapon Formulas'!B21))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
@@ -13310,7 +13649,10 @@
       <c r="T22" s="2">
         <v>0</v>
       </c>
-      <c r="U22" s="2"/>
+      <c r="U22" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C22)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D22+2)*(1+'Weapon Formulas'!B22))</f>
+        <v>-106.66666666666666</v>
+      </c>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
@@ -13384,7 +13726,10 @@
       <c r="T23" s="2">
         <v>0</v>
       </c>
-      <c r="U23" s="2"/>
+      <c r="U23" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C23)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D23+2)*(1+'Weapon Formulas'!B23))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
@@ -13458,7 +13803,10 @@
       <c r="T24" s="2">
         <v>0</v>
       </c>
-      <c r="U24" s="2"/>
+      <c r="U24" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C24)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D24+2)*(1+'Weapon Formulas'!B24))</f>
+        <v>-106.66666666666666</v>
+      </c>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
@@ -13532,7 +13880,10 @@
       <c r="T25" s="2">
         <v>0</v>
       </c>
-      <c r="U25" s="2"/>
+      <c r="U25" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C25)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D25+2)*(1+'Weapon Formulas'!B25))</f>
+        <v>-213.33333333333331</v>
+      </c>
       <c r="W25" s="14" t="s">
         <v>220</v>
       </c>
@@ -13579,7 +13930,7 @@
       <c r="T26" s="2">
         <v>0</v>
       </c>
-      <c r="U26" s="2"/>
+      <c r="U26" s="14"/>
       <c r="W26" s="14" t="s">
         <v>130</v>
       </c>
@@ -13734,7 +14085,10 @@
       <c r="T27" s="2">
         <v>0</v>
       </c>
-      <c r="U27" s="2"/>
+      <c r="U27" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C27)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D27+2)*(1+'Weapon Formulas'!B27))</f>
+        <v>-213.33333333333331</v>
+      </c>
       <c r="W27" s="14" t="s">
         <v>221</v>
       </c>
@@ -13890,7 +14244,10 @@
       <c r="T28" s="2">
         <v>0</v>
       </c>
-      <c r="U28" s="2"/>
+      <c r="U28" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C28)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D28+2)*(1+'Weapon Formulas'!B28))</f>
+        <v>-426.66666666666663</v>
+      </c>
       <c r="W28" s="14" t="s">
         <v>222</v>
       </c>
@@ -14011,7 +14368,7 @@
       <c r="T29" s="2">
         <v>0</v>
       </c>
-      <c r="U29" s="2"/>
+      <c r="U29" s="14"/>
       <c r="W29" s="14" t="s">
         <v>223</v>
       </c>
@@ -14164,7 +14521,10 @@
       <c r="T30" s="2">
         <v>0</v>
       </c>
-      <c r="U30" s="2"/>
+      <c r="U30" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C30)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D30+2)*(1+'Weapon Formulas'!B30))</f>
+        <v>-13.333333333333332</v>
+      </c>
       <c r="W30" s="14" t="s">
         <v>224</v>
       </c>
@@ -14317,7 +14677,10 @@
       <c r="T31" s="2">
         <v>0</v>
       </c>
-      <c r="U31" s="2"/>
+      <c r="U31" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C31)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D31+2)*(1+'Weapon Formulas'!B31))</f>
+        <v>-26.666666666666664</v>
+      </c>
       <c r="W31" s="14" t="s">
         <v>225</v>
       </c>
@@ -14470,7 +14833,10 @@
       <c r="T32" s="2">
         <v>0</v>
       </c>
-      <c r="U32" s="2"/>
+      <c r="U32" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C32)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D32+2)*(1+'Weapon Formulas'!B32))</f>
+        <v>-53.333333333333329</v>
+      </c>
       <c r="W32" s="14" t="s">
         <v>226</v>
       </c>
@@ -14623,7 +14989,10 @@
       <c r="T33" s="2">
         <v>0</v>
       </c>
-      <c r="U33" s="2"/>
+      <c r="U33" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C33)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D33+2)*(1+'Weapon Formulas'!B33))</f>
+        <v>-26.666666666666664</v>
+      </c>
       <c r="W33" s="14" t="s">
         <v>227</v>
       </c>
@@ -14776,7 +15145,10 @@
       <c r="T34" s="2">
         <v>0</v>
       </c>
-      <c r="U34" s="2"/>
+      <c r="U34" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C34)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D34+2)*(1+'Weapon Formulas'!B34))</f>
+        <v>-53.333333333333329</v>
+      </c>
       <c r="W34" s="14" t="s">
         <v>228</v>
       </c>
@@ -14929,7 +15301,10 @@
       <c r="T35" s="2">
         <v>0</v>
       </c>
-      <c r="U35" s="2"/>
+      <c r="U35" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C35)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D35+2)*(1+'Weapon Formulas'!B35))</f>
+        <v>-106.66666666666666</v>
+      </c>
       <c r="W35" s="14" t="s">
         <v>229</v>
       </c>
@@ -15082,7 +15457,10 @@
       <c r="T36" s="2">
         <v>0</v>
       </c>
-      <c r="U36" s="2"/>
+      <c r="U36" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C36)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D36+2)*(1+'Weapon Formulas'!B36))</f>
+        <v>-53.333333333333329</v>
+      </c>
       <c r="W36" s="14" t="s">
         <v>230</v>
       </c>
@@ -15235,7 +15613,10 @@
       <c r="T37" s="2">
         <v>0</v>
       </c>
-      <c r="U37" s="2"/>
+      <c r="U37" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C37)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D37+2)*(1+'Weapon Formulas'!B37))</f>
+        <v>-106.66666666666666</v>
+      </c>
       <c r="W37" s="14" t="s">
         <v>231</v>
       </c>
@@ -15388,7 +15769,10 @@
       <c r="T38" s="2">
         <v>0</v>
       </c>
-      <c r="U38" s="2"/>
+      <c r="U38" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C38)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D38+2)*(1+'Weapon Formulas'!B38))</f>
+        <v>-213.33333333333331</v>
+      </c>
       <c r="W38" s="2"/>
     </row>
     <row r="39" spans="1:42" x14ac:dyDescent="0.25">
@@ -15430,7 +15814,7 @@
       <c r="T39" s="2">
         <v>0</v>
       </c>
-      <c r="U39" s="2"/>
+      <c r="U39" s="14"/>
       <c r="W39" s="2"/>
     </row>
     <row r="40" spans="1:42" x14ac:dyDescent="0.25">
@@ -15508,7 +15892,10 @@
       <c r="T40" s="2">
         <v>0</v>
       </c>
-      <c r="U40" s="2"/>
+      <c r="U40" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C40)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D40+2)*(1+'Weapon Formulas'!B40))</f>
+        <v>-213.33333333333331</v>
+      </c>
       <c r="W40" s="2"/>
     </row>
     <row r="41" spans="1:42" x14ac:dyDescent="0.25">
@@ -15586,7 +15973,10 @@
       <c r="T41" s="2">
         <v>0</v>
       </c>
-      <c r="U41" s="2"/>
+      <c r="U41" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C41)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D41+2)*(1+'Weapon Formulas'!B41))</f>
+        <v>-426.66666666666663</v>
+      </c>
       <c r="W41" s="2"/>
     </row>
     <row r="42" spans="1:42" x14ac:dyDescent="0.25">
@@ -15628,7 +16018,7 @@
       <c r="T42" s="2">
         <v>0</v>
       </c>
-      <c r="U42" s="2"/>
+      <c r="U42" s="14"/>
       <c r="W42" s="2"/>
     </row>
     <row r="43" spans="1:42" x14ac:dyDescent="0.25">
@@ -15703,7 +16093,10 @@
       <c r="T43" s="2">
         <v>0</v>
       </c>
-      <c r="U43" s="2"/>
+      <c r="U43" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C43)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D43)*(1+'Weapon Formulas'!B43))</f>
+        <v>-13.333333333333332</v>
+      </c>
       <c r="W43" s="2"/>
     </row>
     <row r="44" spans="1:42" x14ac:dyDescent="0.25">
@@ -15778,7 +16171,10 @@
       <c r="T44" s="2">
         <v>0</v>
       </c>
-      <c r="U44" s="2"/>
+      <c r="U44" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C44)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D44)*(1+'Weapon Formulas'!B44))</f>
+        <v>-26.666666666666664</v>
+      </c>
       <c r="W44" s="2"/>
     </row>
     <row r="45" spans="1:42" x14ac:dyDescent="0.25">
@@ -15853,7 +16249,10 @@
       <c r="T45" s="2">
         <v>0</v>
       </c>
-      <c r="U45" s="2"/>
+      <c r="U45" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C45)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D45)*(1+'Weapon Formulas'!B45))</f>
+        <v>-53.333333333333329</v>
+      </c>
       <c r="W45" s="2"/>
     </row>
     <row r="46" spans="1:42" x14ac:dyDescent="0.25">
@@ -15928,7 +16327,10 @@
       <c r="T46" s="2">
         <v>0</v>
       </c>
-      <c r="U46" s="2"/>
+      <c r="U46" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C46)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D46)*(1+'Weapon Formulas'!B46))</f>
+        <v>-26.666666666666664</v>
+      </c>
       <c r="W46" s="2"/>
     </row>
     <row r="47" spans="1:42" x14ac:dyDescent="0.25">
@@ -16003,7 +16405,10 @@
       <c r="T47" s="2">
         <v>0</v>
       </c>
-      <c r="U47" s="2"/>
+      <c r="U47" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C47)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D47)*(1+'Weapon Formulas'!B47))</f>
+        <v>-53.333333333333329</v>
+      </c>
       <c r="W47" s="14"/>
     </row>
     <row r="48" spans="1:42" x14ac:dyDescent="0.25">
@@ -16078,7 +16483,10 @@
       <c r="T48" s="2">
         <v>0</v>
       </c>
-      <c r="U48" s="2"/>
+      <c r="U48" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C48)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D48)*(1+'Weapon Formulas'!B48))</f>
+        <v>-106.66666666666666</v>
+      </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="21">
@@ -16152,7 +16560,10 @@
       <c r="T49" s="2">
         <v>0</v>
       </c>
-      <c r="U49" s="2"/>
+      <c r="U49" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C49)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D49)*(1+'Weapon Formulas'!B49))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="21">
@@ -16226,7 +16637,10 @@
       <c r="T50" s="2">
         <v>0</v>
       </c>
-      <c r="U50" s="2"/>
+      <c r="U50" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C50)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D50)*(1+'Weapon Formulas'!B50))</f>
+        <v>-106.66666666666666</v>
+      </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="21">
@@ -16300,7 +16714,10 @@
       <c r="T51" s="2">
         <v>0</v>
       </c>
-      <c r="U51" s="2"/>
+      <c r="U51" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C51)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D51)*(1+'Weapon Formulas'!B51))</f>
+        <v>-213.33333333333331</v>
+      </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="21">
@@ -16341,7 +16758,7 @@
       <c r="T52" s="2">
         <v>0</v>
       </c>
-      <c r="U52" s="2"/>
+      <c r="U52" s="14"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="21">
@@ -16419,7 +16836,10 @@
         <f>INDEX($T$2:$T$6,C53)</f>
         <v>7.5</v>
       </c>
-      <c r="U53" s="2"/>
+      <c r="U53" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C53)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D53+2)*(1+'Weapon Formulas'!B53))</f>
+        <v>-213.33333333333331</v>
+      </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="21">
@@ -16497,7 +16917,10 @@
         <f>INDEX($T$2:$T$6,C54)</f>
         <v>10</v>
       </c>
-      <c r="U54" s="2"/>
+      <c r="U54" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C54)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D54+2)*(1+'Weapon Formulas'!B54))</f>
+        <v>-426.66666666666663</v>
+      </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="21">
@@ -16538,7 +16961,7 @@
       <c r="T55" s="2">
         <v>0</v>
       </c>
-      <c r="U55" s="2"/>
+      <c r="U55" s="14"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="21">
@@ -16611,7 +17034,10 @@
       <c r="T56" s="2">
         <v>0</v>
       </c>
-      <c r="U56" s="2"/>
+      <c r="U56" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C56)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D56+2)*(1+'Weapon Formulas'!B56))</f>
+        <v>-3.333333333333333</v>
+      </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="21">
@@ -16684,7 +17110,10 @@
       <c r="T57" s="2">
         <v>0</v>
       </c>
-      <c r="U57" s="2"/>
+      <c r="U57" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C57)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D57+2)*(1+'Weapon Formulas'!B57))</f>
+        <v>-6.6666666666666661</v>
+      </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="21">
@@ -16757,7 +17186,10 @@
       <c r="T58" s="2">
         <v>0</v>
       </c>
-      <c r="U58" s="2"/>
+      <c r="U58" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C58)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D58+2)*(1+'Weapon Formulas'!B58))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="21">
@@ -16830,7 +17262,10 @@
       <c r="T59" s="2">
         <v>0</v>
       </c>
-      <c r="U59" s="2"/>
+      <c r="U59" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C59)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D59+2)*(1+'Weapon Formulas'!B59))</f>
+        <v>-6.6666666666666661</v>
+      </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="21">
@@ -16903,7 +17338,10 @@
       <c r="T60" s="2">
         <v>0</v>
       </c>
-      <c r="U60" s="2"/>
+      <c r="U60" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C60)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D60+2)*(1+'Weapon Formulas'!B60))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="21">
@@ -16976,7 +17414,10 @@
       <c r="T61" s="2">
         <v>0</v>
       </c>
-      <c r="U61" s="2"/>
+      <c r="U61" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C61)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D61+2)*(1+'Weapon Formulas'!B61))</f>
+        <v>-26.666666666666664</v>
+      </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="21">
@@ -17049,7 +17490,10 @@
       <c r="T62" s="2">
         <v>0</v>
       </c>
-      <c r="U62" s="2"/>
+      <c r="U62" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C62)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D62+2)*(1+'Weapon Formulas'!B62))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="21">
@@ -17122,7 +17566,10 @@
       <c r="T63" s="2">
         <v>0</v>
       </c>
-      <c r="U63" s="2"/>
+      <c r="U63" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C63)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D63+2)*(1+'Weapon Formulas'!B63))</f>
+        <v>-26.666666666666664</v>
+      </c>
       <c r="X63" s="14"/>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
@@ -17196,7 +17643,10 @@
       <c r="T64" s="2">
         <v>0</v>
       </c>
-      <c r="U64" s="2"/>
+      <c r="U64" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C64)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D64+2)*(1+'Weapon Formulas'!B64))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="21">
@@ -17269,7 +17719,10 @@
       <c r="T65" s="2">
         <v>0</v>
       </c>
-      <c r="U65" s="2"/>
+      <c r="U65" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C65)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D65+2)*(1+'Weapon Formulas'!B65))</f>
+        <v>-26.666666666666664</v>
+      </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="21">
@@ -17342,7 +17795,10 @@
       <c r="T66" s="2">
         <v>0</v>
       </c>
-      <c r="U66" s="2"/>
+      <c r="U66" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C66)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D66+2)*(1+'Weapon Formulas'!B66))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="21">
@@ -17415,7 +17871,10 @@
       <c r="T67" s="2">
         <v>0</v>
       </c>
-      <c r="U67" s="2"/>
+      <c r="U67" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C67)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D67+2)*(1+'Weapon Formulas'!B67))</f>
+        <v>-106.66666666666666</v>
+      </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="21">
@@ -17488,7 +17947,10 @@
       <c r="T68" s="2">
         <v>0</v>
       </c>
-      <c r="U68" s="2"/>
+      <c r="U68" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C68)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D68+2)*(1+'Weapon Formulas'!B68))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="21">
@@ -17561,7 +18023,10 @@
       <c r="T69" s="2">
         <v>0</v>
       </c>
-      <c r="U69" s="2"/>
+      <c r="U69" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C69)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D69+2)*(1+'Weapon Formulas'!B69))</f>
+        <v>-106.66666666666666</v>
+      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="21">
@@ -17634,7 +18099,10 @@
       <c r="T70" s="2">
         <v>0</v>
       </c>
-      <c r="U70" s="2"/>
+      <c r="U70" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C70)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D70+2)*(1+'Weapon Formulas'!B70))</f>
+        <v>-213.33333333333331</v>
+      </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="21">
@@ -17671,7 +18139,7 @@
       <c r="T71" s="2">
         <v>0</v>
       </c>
-      <c r="U71" s="2"/>
+      <c r="U71" s="14"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="21">
@@ -17747,7 +18215,10 @@
       <c r="T72" s="2">
         <v>0</v>
       </c>
-      <c r="U72" s="2"/>
+      <c r="U72" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C72)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D72+2)*(1+'Weapon Formulas'!B72))</f>
+        <v>-213.33333333333331</v>
+      </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="21">
@@ -17823,7 +18294,10 @@
       <c r="T73" s="2">
         <v>0</v>
       </c>
-      <c r="U73" s="2"/>
+      <c r="U73" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C73)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D73+2)*(1+'Weapon Formulas'!B73))</f>
+        <v>-426.66666666666663</v>
+      </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="21">
@@ -17860,7 +18334,7 @@
       <c r="T74" s="2">
         <v>0</v>
       </c>
-      <c r="U74" s="2"/>
+      <c r="U74" s="14"/>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="21">
@@ -17933,7 +18407,10 @@
       <c r="T75" s="2">
         <v>0</v>
       </c>
-      <c r="U75" s="2"/>
+      <c r="U75" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C75)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D75+2)*(1+'Weapon Formulas'!B75))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="21">
@@ -18006,7 +18483,10 @@
       <c r="T76" s="2">
         <v>0</v>
       </c>
-      <c r="U76" s="2"/>
+      <c r="U76" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C76)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D76+2)*(1+'Weapon Formulas'!B76))</f>
+        <v>-26.666666666666664</v>
+      </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="21">
@@ -18079,7 +18559,10 @@
       <c r="T77" s="2">
         <v>0</v>
       </c>
-      <c r="U77" s="2"/>
+      <c r="U77" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C77)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D77+2)*(1+'Weapon Formulas'!B77))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="21">
@@ -18152,7 +18635,10 @@
       <c r="T78" s="2">
         <v>0</v>
       </c>
-      <c r="U78" s="2"/>
+      <c r="U78" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C78)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D78+2)*(1+'Weapon Formulas'!B78))</f>
+        <v>-26.666666666666664</v>
+      </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="21">
@@ -18225,7 +18711,10 @@
       <c r="T79" s="2">
         <v>0</v>
       </c>
-      <c r="U79" s="2"/>
+      <c r="U79" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C79)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D79+2)*(1+'Weapon Formulas'!B79))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="21">
@@ -18298,7 +18787,10 @@
       <c r="T80" s="2">
         <v>0</v>
       </c>
-      <c r="U80" s="2"/>
+      <c r="U80" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C80)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D80+2)*(1+'Weapon Formulas'!B80))</f>
+        <v>-106.66666666666666</v>
+      </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="21">
@@ -18371,7 +18863,10 @@
       <c r="T81" s="2">
         <v>0</v>
       </c>
-      <c r="U81" s="2"/>
+      <c r="U81" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C81)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D81+2)*(1+'Weapon Formulas'!B81))</f>
+        <v>-53.333333333333329</v>
+      </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="21">
@@ -18444,7 +18939,10 @@
       <c r="T82" s="2">
         <v>0</v>
       </c>
-      <c r="U82" s="2"/>
+      <c r="U82" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C82)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D82+2)*(1+'Weapon Formulas'!B82))</f>
+        <v>-106.66666666666666</v>
+      </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="21">
@@ -18517,7 +19015,10 @@
       <c r="T83" s="2">
         <v>0</v>
       </c>
-      <c r="U83" s="2"/>
+      <c r="U83" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C83)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D83+2)*(1+'Weapon Formulas'!B83))</f>
+        <v>-213.33333333333331</v>
+      </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="21">
@@ -18552,7 +19053,7 @@
       <c r="T84" s="2">
         <v>0</v>
       </c>
-      <c r="U84" s="2"/>
+      <c r="U84" s="14"/>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="21">
@@ -18621,7 +19122,10 @@
       <c r="T85" s="2">
         <v>0</v>
       </c>
-      <c r="U85" s="2"/>
+      <c r="U85" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C85)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D85+2)*(1+'Weapon Formulas'!B85))</f>
+        <v>-106.66666666666666</v>
+      </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="21">
@@ -18689,7 +19193,10 @@
       <c r="T86" s="2">
         <v>0</v>
       </c>
-      <c r="U86" s="2"/>
+      <c r="U86" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C86)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D86+2)*(1+'Weapon Formulas'!B86))</f>
+        <v>-213.33333333333331</v>
+      </c>
     </row>
     <row r="87" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="21">
@@ -18805,7 +19312,10 @@
         <f>INDEX($T$2:$T$6,C88)</f>
         <v>2.5</v>
       </c>
-      <c r="U88" s="2"/>
+      <c r="U88" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C88)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D88+2)*(1+'Weapon Formulas'!B88))</f>
+        <v>-3.333333333333333</v>
+      </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="21">
@@ -18879,7 +19389,10 @@
         <f t="shared" ref="T89:T115" si="72">INDEX($T$2:$T$6,C89)</f>
         <v>2.5</v>
       </c>
-      <c r="U89" s="2"/>
+      <c r="U89" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C89)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D89+2)*(1+'Weapon Formulas'!B89))</f>
+        <v>-6.6666666666666661</v>
+      </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="21">
@@ -18953,7 +19466,10 @@
         <f t="shared" si="72"/>
         <v>2.5</v>
       </c>
-      <c r="U90" s="2"/>
+      <c r="U90" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C90)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D90+2)*(1+'Weapon Formulas'!B90))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="21">
@@ -19027,7 +19543,10 @@
         <f t="shared" si="72"/>
         <v>3.75</v>
       </c>
-      <c r="U91" s="2"/>
+      <c r="U91" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C91)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D91+2)*(1+'Weapon Formulas'!B91))</f>
+        <v>-6.6666666666666661</v>
+      </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="21">
@@ -19101,7 +19620,10 @@
         <f t="shared" si="72"/>
         <v>3.75</v>
       </c>
-      <c r="U92" s="2"/>
+      <c r="U92" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C92)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D92+2)*(1+'Weapon Formulas'!B92))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="21">
@@ -19175,7 +19697,10 @@
         <f t="shared" si="72"/>
         <v>3.75</v>
       </c>
-      <c r="U93" s="2"/>
+      <c r="U93" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C93)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D93+2)*(1+'Weapon Formulas'!B93))</f>
+        <v>-26.666666666666664</v>
+      </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="21">
@@ -19249,7 +19774,10 @@
         <f t="shared" si="72"/>
         <v>5</v>
       </c>
-      <c r="U94" s="2"/>
+      <c r="U94" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C94)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D94+2)*(1+'Weapon Formulas'!B94))</f>
+        <v>-13.333333333333332</v>
+      </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="21">
@@ -19323,7 +19851,10 @@
         <f t="shared" si="72"/>
         <v>5</v>
       </c>
-      <c r="U95" s="2"/>
+      <c r="U95" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C95)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D95+2)*(1+'Weapon Formulas'!B95))</f>
+        <v>-26.666666666666664</v>
+      </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="21">
@@ -19397,9 +19928,12 @@
         <f t="shared" si="72"/>
         <v>5</v>
       </c>
-      <c r="U96" s="2"/>
-    </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U96" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C96)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D96+2)*(1+'Weapon Formulas'!B96))</f>
+        <v>-53.333333333333329</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="21">
         <f t="shared" si="61"/>
         <v>-9.0000000000000011E-3</v>
@@ -19471,9 +20005,12 @@
         <f t="shared" si="72"/>
         <v>7.5</v>
       </c>
-      <c r="U97" s="2"/>
-    </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U97" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C97)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D97+2)*(1+'Weapon Formulas'!B97))</f>
+        <v>-26.666666666666664</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -19545,9 +20082,12 @@
         <f t="shared" si="72"/>
         <v>7.5</v>
       </c>
-      <c r="U98" s="2"/>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U98" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C98)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D98+2)*(1+'Weapon Formulas'!B98))</f>
+        <v>-53.333333333333329</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="21">
         <f t="shared" si="61"/>
         <v>-8.1000000000000003E-2</v>
@@ -19619,9 +20159,12 @@
         <f t="shared" si="72"/>
         <v>7.5</v>
       </c>
-      <c r="U99" s="2"/>
-    </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U99" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C99)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D99+2)*(1+'Weapon Formulas'!B99))</f>
+        <v>-106.66666666666666</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="21">
         <f t="shared" si="61"/>
         <v>-9.0000000000000011E-3</v>
@@ -19693,9 +20236,12 @@
         <f t="shared" si="72"/>
         <v>10</v>
       </c>
-      <c r="U100" s="2"/>
-    </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U100" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C100)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D100+2)*(1+'Weapon Formulas'!B100))</f>
+        <v>-53.333333333333329</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -19767,9 +20313,12 @@
         <f t="shared" si="72"/>
         <v>10</v>
       </c>
-      <c r="U101" s="2"/>
-    </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U101" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C101)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D101+2)*(1+'Weapon Formulas'!B101))</f>
+        <v>-106.66666666666666</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="21">
         <f t="shared" si="61"/>
         <v>-8.1000000000000003E-2</v>
@@ -19841,9 +20390,12 @@
         <f t="shared" si="72"/>
         <v>10</v>
       </c>
-      <c r="U102" s="2"/>
-    </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U102" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C102)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D102+2)*(1+'Weapon Formulas'!B102))</f>
+        <v>-213.33333333333331</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -19882,9 +20434,9 @@
       <c r="T103" s="2">
         <v>0</v>
       </c>
-      <c r="U103" s="2"/>
-    </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U103" s="14"/>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="21">
         <f t="shared" si="61"/>
         <v>-9.0000000000000011E-3</v>
@@ -19956,13 +20508,12 @@
         <f t="shared" si="72"/>
         <v>5</v>
       </c>
-      <c r="U104" s="2"/>
-      <c r="W104">
-        <f>LOG(10,5)</f>
-        <v>1.4306765580733933</v>
-      </c>
-    </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U104" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C104)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D104+2)*(1+'Weapon Formulas'!B104))</f>
+        <v>-13.333333333333332</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -20034,9 +20585,12 @@
         <f t="shared" si="72"/>
         <v>5</v>
       </c>
-      <c r="U105" s="2"/>
-    </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U105" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C105)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D105+2)*(1+'Weapon Formulas'!B105))</f>
+        <v>-26.666666666666664</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="21">
         <f t="shared" si="61"/>
         <v>-8.1000000000000003E-2</v>
@@ -20108,9 +20662,12 @@
         <f t="shared" si="72"/>
         <v>5</v>
       </c>
-      <c r="U106" s="2"/>
-    </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U106" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C106)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D106+2)*(1+'Weapon Formulas'!B106))</f>
+        <v>-53.333333333333329</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="21">
         <f t="shared" si="61"/>
         <v>-9.0000000000000011E-3</v>
@@ -20182,9 +20739,12 @@
         <f t="shared" si="72"/>
         <v>7.5</v>
       </c>
-      <c r="U107" s="2"/>
-    </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U107" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C107)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D107+2)*(1+'Weapon Formulas'!B107))</f>
+        <v>-26.666666666666664</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -20256,9 +20816,12 @@
         <f t="shared" si="72"/>
         <v>7.5</v>
       </c>
-      <c r="U108" s="2"/>
-    </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U108" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C108)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D108+2)*(1+'Weapon Formulas'!B108))</f>
+        <v>-53.333333333333329</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" s="21">
         <f t="shared" si="61"/>
         <v>-8.1000000000000003E-2</v>
@@ -20330,9 +20893,12 @@
         <f t="shared" si="72"/>
         <v>7.5</v>
       </c>
-      <c r="U109" s="2"/>
-    </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U109" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C109)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D109+2)*(1+'Weapon Formulas'!B109))</f>
+        <v>-106.66666666666666</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="21">
         <f t="shared" si="61"/>
         <v>-9.0000000000000011E-3</v>
@@ -20404,9 +20970,12 @@
         <f t="shared" si="72"/>
         <v>10</v>
       </c>
-      <c r="U110" s="2"/>
-    </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U110" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C110)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D110+2)*(1+'Weapon Formulas'!B110))</f>
+        <v>-53.333333333333329</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -20478,9 +21047,12 @@
         <f t="shared" si="72"/>
         <v>10</v>
       </c>
-      <c r="U111" s="2"/>
-    </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U111" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C111)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D111+2)*(1+'Weapon Formulas'!B111))</f>
+        <v>-106.66666666666666</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="21">
         <f t="shared" si="61"/>
         <v>-8.1000000000000003E-2</v>
@@ -20552,8 +21124,12 @@
         <f t="shared" si="72"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U112" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C112)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D112+2)*(1+'Weapon Formulas'!B112))</f>
+        <v>-213.33333333333331</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -20591,8 +21167,9 @@
         <v>60</v>
       </c>
       <c r="T113" s="2"/>
-    </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U113" s="14"/>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -20667,8 +21244,12 @@
         <f t="shared" si="72"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U114" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C114)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D114+2)*(1+'Weapon Formulas'!B114))</f>
+        <v>-106.66666666666666</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -20743,8 +21324,12 @@
         <f t="shared" si="72"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U115" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C115)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D115+2)*(1+'Weapon Formulas'!B115))</f>
+        <v>-213.33333333333331</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="21">
         <f t="shared" si="61"/>
         <v>-4.4999999999999998E-2</v>
@@ -20782,8 +21367,9 @@
         <v>60</v>
       </c>
       <c r="T116" s="2"/>
-    </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U116" s="14"/>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" s="21">
         <f t="shared" si="61"/>
         <v>-8.1000000000000003E-2</v>
@@ -20855,8 +21441,12 @@
       <c r="T117" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U117" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C117)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D117+2)*(1+'Weapon Formulas'!B117))</f>
+        <v>-106.66666666666666</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" s="21">
         <f t="shared" si="61"/>
         <v>-8.1000000000000003E-2</v>
@@ -20928,8 +21518,12 @@
       <c r="T118" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U118" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C118)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D118+2)*(1+'Weapon Formulas'!B118))</f>
+        <v>-213.33333333333331</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" s="21">
         <f t="shared" si="61"/>
         <v>-8.1000000000000003E-2</v>
@@ -21001,8 +21595,12 @@
       <c r="T119" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U119" s="14">
+        <f>-INDEX('Ship Design Balancing'!$K$2:$K$6,'Weapon Formulas'!C119)*(INDEX('Weapon Formulas'!$R$1:$R$3,'Weapon Formulas'!D119+2)*(1+'Weapon Formulas'!B119))</f>
+        <v>-426.66666666666663</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K120" s="13" t="s">
         <v>142</v>
       </c>
@@ -21031,7 +21629,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L121" s="13"/>
       <c r="M121"/>
     </row>
@@ -21047,32 +21645,164 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I13"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I13">
-        <f>64/3</f>
-        <v>21.333333333333332</v>
+      <c r="C1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="I2" s="14">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <f>2/3*J2</f>
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f>J2*2</f>
+        <v>10</v>
+      </c>
+      <c r="K3" s="22">
+        <f t="shared" ref="K3:K6" si="0">2/3*J3</f>
+        <v>6.6666666666666661</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4">
+        <f>B3/4</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="22">
+        <f t="shared" ref="C4:E4" si="1">C3/4</f>
+        <v>4</v>
+      </c>
+      <c r="D4" s="22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E4" s="22">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" s="22">
+        <f t="shared" ref="J4:J6" si="2">J3*2</f>
+        <v>20</v>
+      </c>
+      <c r="K4" s="22">
+        <f t="shared" si="0"/>
+        <v>13.333333333333332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" s="22">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="K5" s="22">
+        <f t="shared" si="0"/>
+        <v>26.666666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="22">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="K6" s="22">
+        <f t="shared" si="0"/>
+        <v>53.333333333333329</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21080,8 +21810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U179"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="U108" sqref="U108"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21183,7 +21913,7 @@
         <v>146</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="23"/>
+      <c r="P4" s="24"/>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -21212,7 +21942,7 @@
         <v>147</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="24"/>
+      <c r="P5" s="25"/>
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -21261,7 +21991,7 @@
       <c r="O6" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="P6" s="24"/>
+      <c r="P6" s="25"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -21282,7 +22012,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="24"/>
+      <c r="P7" s="25"/>
       <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -21293,7 +22023,8 @@
         <v>2.5</v>
       </c>
       <c r="C8" s="5">
-        <v>-2.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A8,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C8),2)</f>
+        <v>-3.33</v>
       </c>
       <c r="D8" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A8,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D8),2)</f>
@@ -21347,7 +22078,8 @@
         <v>5</v>
       </c>
       <c r="C9" s="5">
-        <v>-5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A9,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C9),2)</f>
+        <v>-6.67</v>
       </c>
       <c r="D9" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A9,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D9),2)</f>
@@ -21401,7 +22133,8 @@
         <v>10</v>
       </c>
       <c r="C10" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A10,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C10),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D10" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A10,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D10),2)</f>
@@ -21455,7 +22188,8 @@
         <v>5</v>
       </c>
       <c r="C11" s="5">
-        <v>-5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A11,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C11),2)</f>
+        <v>-6.67</v>
       </c>
       <c r="D11" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A11,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D11),2)</f>
@@ -21509,7 +22243,8 @@
         <v>10</v>
       </c>
       <c r="C12" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A12,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C12),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D12" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A12,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D12),2)</f>
@@ -21563,7 +22298,8 @@
         <v>20</v>
       </c>
       <c r="C13" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A13,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C13),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D13" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A13,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D13),2)</f>
@@ -21617,7 +22353,8 @@
         <v>7.5</v>
       </c>
       <c r="C14" s="5">
-        <v>-7.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A14,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C14),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D14" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A14,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D14),2)</f>
@@ -21671,7 +22408,8 @@
         <v>15</v>
       </c>
       <c r="C15" s="5">
-        <v>-15</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A15,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C15),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D15" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A15,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D15),2)</f>
@@ -21725,7 +22463,8 @@
         <v>30</v>
       </c>
       <c r="C16" s="5">
-        <v>-30</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A16,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C16),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D16" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A16,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D16),2)</f>
@@ -21779,7 +22518,8 @@
         <v>10</v>
       </c>
       <c r="C17" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A17,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C17),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D17" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A17,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D17),2)</f>
@@ -21833,7 +22573,8 @@
         <v>20</v>
       </c>
       <c r="C18" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A18,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C18),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D18" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A18,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D18),2)</f>
@@ -21887,7 +22628,8 @@
         <v>40</v>
       </c>
       <c r="C19" s="5">
-        <v>-40</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A19,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C19),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D19" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A19,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D19),2)</f>
@@ -21941,7 +22683,8 @@
         <v>12.5</v>
       </c>
       <c r="C20" s="5">
-        <v>-12.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A20,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C20),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D20" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A20,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D20),2)</f>
@@ -21995,7 +22738,8 @@
         <v>25</v>
       </c>
       <c r="C21" s="5">
-        <v>-25</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A21,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C21),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D21" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A21,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D21),2)</f>
@@ -22049,7 +22793,8 @@
         <v>50</v>
       </c>
       <c r="C22" s="5">
-        <v>-50</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A22,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C22),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D22" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A22,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D22),2)</f>
@@ -22100,7 +22845,7 @@
         <v>150</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -22124,6 +22869,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A24,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C24),2)</f>
         <v>0</v>
       </c>
       <c r="D24" s="5">
@@ -22178,6 +22924,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A25,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C25),2)</f>
         <v>0</v>
       </c>
       <c r="D25" s="5">
@@ -22231,7 +22978,8 @@
       <c r="B26" s="2">
         <v>0</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A26,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C26),2)</f>
         <v>0</v>
       </c>
       <c r="D26" s="5">
@@ -22307,7 +23055,8 @@
         <v>100</v>
       </c>
       <c r="C28" s="5">
-        <v>-100</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A28,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C28),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D28" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A28,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D28),2)</f>
@@ -22361,7 +23110,8 @@
         <v>120</v>
       </c>
       <c r="C29" s="5">
-        <v>-120</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A29,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C29),2)</f>
+        <v>-426.67</v>
       </c>
       <c r="D29" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A29,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D29),2)</f>
@@ -22436,7 +23186,8 @@
         <v>7.5</v>
       </c>
       <c r="C31" s="5">
-        <v>-7.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A31,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C31),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D31" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A31,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D31),2)</f>
@@ -22490,7 +23241,8 @@
         <v>15</v>
       </c>
       <c r="C32" s="5">
-        <v>-15</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A32,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C32),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D32" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A32,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D32),2)</f>
@@ -22544,7 +23296,8 @@
         <v>30</v>
       </c>
       <c r="C33" s="5">
-        <v>-30</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A33,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C33),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D33" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A33,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D33),2)</f>
@@ -22598,7 +23351,8 @@
         <v>10</v>
       </c>
       <c r="C34" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A34,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C34),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D34" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A34,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D34),2)</f>
@@ -22652,7 +23406,8 @@
         <v>20</v>
       </c>
       <c r="C35" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A35,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C35),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D35" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A35,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D35),2)</f>
@@ -22705,8 +23460,9 @@
       <c r="B36" s="2">
         <v>40</v>
       </c>
-      <c r="C36" s="2">
-        <v>-40</v>
+      <c r="C36" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A36,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C36),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D36" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A36,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D36),2)</f>
@@ -22760,7 +23516,8 @@
         <v>12.5</v>
       </c>
       <c r="C37" s="5">
-        <v>-12.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A37,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C37),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D37" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A37,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D37),2)</f>
@@ -22814,7 +23571,8 @@
         <v>25</v>
       </c>
       <c r="C38" s="5">
-        <v>-25</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A38,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C38),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D38" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A38,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D38),2)</f>
@@ -22867,8 +23625,9 @@
       <c r="B39" s="2">
         <v>50</v>
       </c>
-      <c r="C39" s="2">
-        <v>-50</v>
+      <c r="C39" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A39,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C39),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D39" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A39,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D39),2)</f>
@@ -22943,7 +23702,8 @@
         <v>100</v>
       </c>
       <c r="C41" s="5">
-        <v>-100</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A41,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C41),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D41" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A41,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D41),2)</f>
@@ -22997,7 +23757,8 @@
         <v>120</v>
       </c>
       <c r="C42" s="5">
-        <v>-120</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A42,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C42),2)</f>
+        <v>-426.67</v>
       </c>
       <c r="D42" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A42,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D42),2)</f>
@@ -23072,7 +23833,8 @@
         <v>7.5</v>
       </c>
       <c r="C44" s="5">
-        <v>-7.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A44,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C44),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D44" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A44,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D44),2)</f>
@@ -23126,7 +23888,8 @@
         <v>15</v>
       </c>
       <c r="C45" s="5">
-        <v>-15</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A45,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C45),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D45" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A45,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D45),2)</f>
@@ -23180,7 +23943,8 @@
         <v>30</v>
       </c>
       <c r="C46" s="5">
-        <v>-30</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A46,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C46),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D46" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A46,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D46),2)</f>
@@ -23234,7 +23998,8 @@
         <v>10</v>
       </c>
       <c r="C47" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A47,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C47),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D47" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A47,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D47),2)</f>
@@ -23288,7 +24053,8 @@
         <v>20</v>
       </c>
       <c r="C48" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A48,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C48),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D48" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A48,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D48),2)</f>
@@ -23341,8 +24107,9 @@
       <c r="B49" s="2">
         <v>40</v>
       </c>
-      <c r="C49" s="2">
-        <v>-40</v>
+      <c r="C49" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A49,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C49),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D49" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A49,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D49),2)</f>
@@ -23396,7 +24163,8 @@
         <v>12.5</v>
       </c>
       <c r="C50" s="5">
-        <v>-12.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A50,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C50),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D50" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A50,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D50),2)</f>
@@ -23450,7 +24218,8 @@
         <v>25</v>
       </c>
       <c r="C51" s="5">
-        <v>-25</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A51,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C51),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D51" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A51,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D51),2)</f>
@@ -23503,8 +24272,9 @@
       <c r="B52" s="2">
         <v>50</v>
       </c>
-      <c r="C52" s="2">
-        <v>-50</v>
+      <c r="C52" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A52,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C52),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D52" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A52,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D52),2)</f>
@@ -23579,7 +24349,8 @@
         <v>100</v>
       </c>
       <c r="C54" s="5">
-        <v>-100</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A54,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C54),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D54" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A54,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D54),2)</f>
@@ -23633,7 +24404,8 @@
         <v>120</v>
       </c>
       <c r="C55" s="5">
-        <v>-120</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A55,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C55),2)</f>
+        <v>-426.67</v>
       </c>
       <c r="D55" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A55,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D55),2)</f>
@@ -23708,7 +24480,8 @@
         <v>2.5</v>
       </c>
       <c r="C57" s="5">
-        <v>-2.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A57,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C57),2)</f>
+        <v>-3.33</v>
       </c>
       <c r="D57" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A57,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D57),2)</f>
@@ -23762,7 +24535,8 @@
         <v>5</v>
       </c>
       <c r="C58" s="5">
-        <v>-5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A58,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C58),2)</f>
+        <v>-6.67</v>
       </c>
       <c r="D58" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A58,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D58),2)</f>
@@ -23816,7 +24590,8 @@
         <v>10</v>
       </c>
       <c r="C59" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A59,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C59),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D59" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A59,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D59),2)</f>
@@ -23870,7 +24645,8 @@
         <v>5</v>
       </c>
       <c r="C60" s="5">
-        <v>-5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A60,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C60),2)</f>
+        <v>-6.67</v>
       </c>
       <c r="D60" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A60,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D60),2)</f>
@@ -23924,7 +24700,8 @@
         <v>10</v>
       </c>
       <c r="C61" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A61,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C61),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D61" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A61,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D61),2)</f>
@@ -23978,7 +24755,8 @@
         <v>20</v>
       </c>
       <c r="C62" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A62,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C62),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D62" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A62,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D62),2)</f>
@@ -24032,7 +24810,8 @@
         <v>7.5</v>
       </c>
       <c r="C63" s="5">
-        <v>-7.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A63,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C63),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D63" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A63,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D63),2)</f>
@@ -24086,7 +24865,8 @@
         <v>15</v>
       </c>
       <c r="C64" s="5">
-        <v>-15</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A64,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C64),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D64" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A64,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D64),2)</f>
@@ -24140,7 +24920,8 @@
         <v>30</v>
       </c>
       <c r="C65" s="5">
-        <v>-30</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A65,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C65),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D65" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A65,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D65),2)</f>
@@ -24194,7 +24975,8 @@
         <v>10</v>
       </c>
       <c r="C66" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A66,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C66),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D66" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A66,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D66),2)</f>
@@ -24248,7 +25030,8 @@
         <v>20</v>
       </c>
       <c r="C67" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A67,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C67),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D67" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A67,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D67),2)</f>
@@ -24301,8 +25084,9 @@
       <c r="B68" s="2">
         <v>40</v>
       </c>
-      <c r="C68" s="2">
-        <v>-40</v>
+      <c r="C68" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A68,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C68),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D68" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A68,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D68),2)</f>
@@ -24356,7 +25140,8 @@
         <v>12.5</v>
       </c>
       <c r="C69" s="5">
-        <v>-12.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A69,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C69),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D69" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A69,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D69),2)</f>
@@ -24410,7 +25195,8 @@
         <v>25</v>
       </c>
       <c r="C70" s="5">
-        <v>-25</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A70,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C70),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D70" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A70,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D70),2)</f>
@@ -24463,8 +25249,9 @@
       <c r="B71" s="2">
         <v>50</v>
       </c>
-      <c r="C71" s="2">
-        <v>-50</v>
+      <c r="C71" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A71,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C71),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D71" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A71,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D71),2)</f>
@@ -24539,6 +25326,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A73,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C73),2)</f>
         <v>0</v>
       </c>
       <c r="D73" s="5">
@@ -24593,6 +25381,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A74,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C74),2)</f>
         <v>0</v>
       </c>
       <c r="D74" s="5">
@@ -24647,6 +25436,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A75,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C75),2)</f>
         <v>0</v>
       </c>
       <c r="D75" s="5">
@@ -24722,7 +25512,8 @@
         <v>100</v>
       </c>
       <c r="C77" s="5">
-        <v>-100</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A77,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C77),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D77" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A77,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D77),2)</f>
@@ -24776,7 +25567,8 @@
         <v>120</v>
       </c>
       <c r="C78" s="5">
-        <v>-120</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A78,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C78),2)</f>
+        <v>-426.67</v>
       </c>
       <c r="D78" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A78,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D78),2)</f>
@@ -24851,7 +25643,8 @@
         <v>5</v>
       </c>
       <c r="C80" s="5">
-        <v>-5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A80,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C80),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D80" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A80,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D80),2)</f>
@@ -24904,8 +25697,9 @@
       <c r="B81" s="2">
         <v>10</v>
       </c>
-      <c r="C81" s="2">
-        <v>-10</v>
+      <c r="C81" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A81,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C81),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D81" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A81,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D81),2)</f>
@@ -24959,7 +25753,8 @@
         <v>20</v>
       </c>
       <c r="C82" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A82,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C82),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D82" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A82,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D82),2)</f>
@@ -25013,7 +25808,8 @@
         <v>7.5</v>
       </c>
       <c r="C83" s="5">
-        <v>-7.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A83,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C83),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D83" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A83,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D83),2)</f>
@@ -25066,8 +25862,9 @@
       <c r="B84" s="2">
         <v>15</v>
       </c>
-      <c r="C84" s="2">
-        <v>-15</v>
+      <c r="C84" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A84,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C84),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D84" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A84,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D84),2)</f>
@@ -25121,7 +25918,8 @@
         <v>30</v>
       </c>
       <c r="C85" s="5">
-        <v>-30</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A85,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C85),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D85" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A85,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D85),2)</f>
@@ -25175,7 +25973,8 @@
         <v>10</v>
       </c>
       <c r="C86" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A86,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C86),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D86" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A86,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D86),2)</f>
@@ -25229,7 +26028,8 @@
         <v>20</v>
       </c>
       <c r="C87" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A87,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C87),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D87" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A87,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D87),2)</f>
@@ -25283,7 +26083,8 @@
         <v>40</v>
       </c>
       <c r="C88" s="5">
-        <v>-40</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A88,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C88),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D88" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A88,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D88),2)</f>
@@ -25358,7 +26159,8 @@
         <v>50</v>
       </c>
       <c r="C90" s="5">
-        <v>-50</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A90,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C90),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D90" s="5">
         <v>2</v>
@@ -25409,7 +26211,8 @@
         <v>60</v>
       </c>
       <c r="C91" s="5">
-        <v>-60</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A91,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C91),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D91" s="5">
         <v>2</v>
@@ -25482,7 +26285,8 @@
         <v>2.5</v>
       </c>
       <c r="C93" s="5">
-        <v>-2.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A93,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C93),2)</f>
+        <v>-3.33</v>
       </c>
       <c r="D93" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A93,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D93),2)</f>
@@ -25536,7 +26340,8 @@
         <v>5</v>
       </c>
       <c r="C94" s="5">
-        <v>-5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A94,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C94),2)</f>
+        <v>-6.67</v>
       </c>
       <c r="D94" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A94,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D94),2)</f>
@@ -25590,7 +26395,8 @@
         <v>10</v>
       </c>
       <c r="C95" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A95,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C95),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D95" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A95,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D95),2)</f>
@@ -25644,7 +26450,8 @@
         <v>5</v>
       </c>
       <c r="C96" s="5">
-        <v>-5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A96,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C96),2)</f>
+        <v>-6.67</v>
       </c>
       <c r="D96" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A96,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D96),2)</f>
@@ -25698,7 +26505,8 @@
         <v>10</v>
       </c>
       <c r="C97" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A97,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C97),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D97" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A97,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D97),2)</f>
@@ -25752,7 +26560,8 @@
         <v>20</v>
       </c>
       <c r="C98" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A98,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C98),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D98" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A98,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D98),2)</f>
@@ -25806,7 +26615,8 @@
         <v>7.5</v>
       </c>
       <c r="C99" s="5">
-        <v>-7.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A99,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C99),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D99" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A99,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D99),2)</f>
@@ -25859,8 +26669,9 @@
       <c r="B100" s="2">
         <v>15</v>
       </c>
-      <c r="C100" s="2">
-        <v>-15</v>
+      <c r="C100" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A100,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C100),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D100" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A100,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D100),2)</f>
@@ -25914,7 +26725,8 @@
         <v>30</v>
       </c>
       <c r="C101" s="5">
-        <v>-30</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A101,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C101),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D101" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A101,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D101),2)</f>
@@ -25968,7 +26780,8 @@
         <v>10</v>
       </c>
       <c r="C102" s="5">
-        <v>-10</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A102,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C102),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D102" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A102,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D102),2)</f>
@@ -26022,7 +26835,8 @@
         <v>20</v>
       </c>
       <c r="C103" s="5">
-        <v>-20</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A103,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C103),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D103" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A103,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D103),2)</f>
@@ -26076,7 +26890,8 @@
         <v>40</v>
       </c>
       <c r="C104" s="5">
-        <v>-40</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A104,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C104),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D104" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A104,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D104),2)</f>
@@ -26130,7 +26945,8 @@
         <v>12.5</v>
       </c>
       <c r="C105" s="5">
-        <v>-12.5</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A105,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C105),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D105" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A105,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D105),2)</f>
@@ -26184,7 +27000,8 @@
         <v>25</v>
       </c>
       <c r="C106" s="5">
-        <v>-25</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A106,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C106),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D106" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A106,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D106),2)</f>
@@ -26238,7 +27055,8 @@
         <v>50</v>
       </c>
       <c r="C107" s="5">
-        <v>-50</v>
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A107,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C107),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D107" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A107,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D107),2)</f>
@@ -26317,6 +27135,7 @@
         <v>0</v>
       </c>
       <c r="C109" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A109,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C109),2)</f>
         <v>0</v>
       </c>
       <c r="D109" s="5">
@@ -26370,7 +27189,8 @@
       <c r="B110" s="2">
         <v>0</v>
       </c>
-      <c r="C110" s="2">
+      <c r="C110" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A110,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C110),2)</f>
         <v>0</v>
       </c>
       <c r="D110" s="5">
@@ -26425,6 +27245,7 @@
         <v>0</v>
       </c>
       <c r="C111" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A111,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C111),2)</f>
         <v>0</v>
       </c>
       <c r="D111" s="5">
@@ -26499,8 +27320,9 @@
       <c r="B113">
         <v>7.5</v>
       </c>
-      <c r="C113">
-        <v>-7.5</v>
+      <c r="C113" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A113,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C113),2)</f>
+        <v>-13.33</v>
       </c>
       <c r="D113" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A113,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D113),2)</f>
@@ -26550,8 +27372,9 @@
       <c r="B114">
         <v>15</v>
       </c>
-      <c r="C114">
-        <v>-15</v>
+      <c r="C114" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A114,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C114),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D114" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A114,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D114),2)</f>
@@ -26601,8 +27424,9 @@
       <c r="B115">
         <v>30</v>
       </c>
-      <c r="C115">
-        <v>-30</v>
+      <c r="C115" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A115,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C115),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D115" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A115,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D115),2)</f>
@@ -26652,8 +27476,9 @@
       <c r="B116">
         <v>10</v>
       </c>
-      <c r="C116">
-        <v>-10</v>
+      <c r="C116" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A116,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C116),2)</f>
+        <v>-26.67</v>
       </c>
       <c r="D116" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A116,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D116),2)</f>
@@ -26703,8 +27528,9 @@
       <c r="B117">
         <v>20</v>
       </c>
-      <c r="C117">
-        <v>-20</v>
+      <c r="C117" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A117,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C117),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D117" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A117,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D117),2)</f>
@@ -26754,8 +27580,9 @@
       <c r="B118">
         <v>40</v>
       </c>
-      <c r="C118">
-        <v>-40</v>
+      <c r="C118" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A118,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C118),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D118" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A118,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D118),2)</f>
@@ -26805,8 +27632,9 @@
       <c r="B119">
         <v>12.5</v>
       </c>
-      <c r="C119">
-        <v>-12.5</v>
+      <c r="C119" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A119,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C119),2)</f>
+        <v>-53.33</v>
       </c>
       <c r="D119" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A119,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D119),2)</f>
@@ -26856,8 +27684,9 @@
       <c r="B120">
         <v>25</v>
       </c>
-      <c r="C120">
-        <v>-25</v>
+      <c r="C120" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A120,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C120),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D120" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A120,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D120),2)</f>
@@ -26907,8 +27736,9 @@
       <c r="B121">
         <v>50</v>
       </c>
-      <c r="C121">
-        <v>-50</v>
+      <c r="C121" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A121,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C121),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D121" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A121,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D121),2)</f>
@@ -26955,6 +27785,7 @@
       <c r="A122" s="15" t="s">
         <v>126</v>
       </c>
+      <c r="C122" s="5"/>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
@@ -26970,8 +27801,9 @@
       <c r="B123">
         <v>40</v>
       </c>
-      <c r="C123">
-        <v>-40</v>
+      <c r="C123" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A123,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C123),2)</f>
+        <v>-106.67</v>
       </c>
       <c r="D123" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A123,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D123),2)</f>
@@ -27021,8 +27853,9 @@
       <c r="B124">
         <v>50</v>
       </c>
-      <c r="C124">
-        <v>-50</v>
+      <c r="C124" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A124,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C124),2)</f>
+        <v>-213.33</v>
       </c>
       <c r="D124" s="5">
         <f>ROUND(_xlfn.IFNA(VLOOKUP(A124,'Weapon Formulas'!$E$10:$Q$115,11,0),weapon_components!D124),2)</f>
@@ -27069,6 +27902,7 @@
       <c r="A125" s="15" t="s">
         <v>161</v>
       </c>
+      <c r="C125" s="5"/>
       <c r="D125" s="5"/>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
@@ -27084,7 +27918,8 @@
       <c r="B126">
         <v>5</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A126,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C126),2)</f>
         <v>-5</v>
       </c>
       <c r="D126" s="5">
@@ -27135,7 +27970,8 @@
       <c r="B127">
         <v>20</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A127,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C127),2)</f>
         <v>-20</v>
       </c>
       <c r="D127" s="5">
@@ -27183,6 +28019,7 @@
       <c r="A128" s="15" t="s">
         <v>164</v>
       </c>
+      <c r="C128" s="5"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
@@ -27198,7 +28035,8 @@
       <c r="B129">
         <v>2.5</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A129,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C129),2)</f>
         <v>-2.5</v>
       </c>
       <c r="D129" s="5">
@@ -27249,7 +28087,8 @@
       <c r="B130">
         <v>5</v>
       </c>
-      <c r="C130">
+      <c r="C130" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A130,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C130),2)</f>
         <v>-5</v>
       </c>
       <c r="D130" s="5">
@@ -27300,7 +28139,8 @@
       <c r="B131">
         <v>10</v>
       </c>
-      <c r="C131">
+      <c r="C131" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A131,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C131),2)</f>
         <v>-10</v>
       </c>
       <c r="D131" s="5">
@@ -27351,7 +28191,8 @@
       <c r="B132">
         <v>5</v>
       </c>
-      <c r="C132">
+      <c r="C132" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A132,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C132),2)</f>
         <v>-5</v>
       </c>
       <c r="D132" s="5">
@@ -27402,7 +28243,8 @@
       <c r="B133">
         <v>10</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A133,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C133),2)</f>
         <v>-10</v>
       </c>
       <c r="D133" s="5">
@@ -27453,7 +28295,8 @@
       <c r="B134">
         <v>20</v>
       </c>
-      <c r="C134">
+      <c r="C134" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A134,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C134),2)</f>
         <v>-20</v>
       </c>
       <c r="D134" s="5">
@@ -27504,7 +28347,8 @@
       <c r="B135">
         <v>7.5</v>
       </c>
-      <c r="C135">
+      <c r="C135" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A135,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C135),2)</f>
         <v>-7.5</v>
       </c>
       <c r="D135" s="5">
@@ -27555,7 +28399,8 @@
       <c r="B136">
         <v>15</v>
       </c>
-      <c r="C136">
+      <c r="C136" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A136,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C136),2)</f>
         <v>-15</v>
       </c>
       <c r="D136" s="5">
@@ -27606,7 +28451,8 @@
       <c r="B137">
         <v>30</v>
       </c>
-      <c r="C137">
+      <c r="C137" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A137,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C137),2)</f>
         <v>-30</v>
       </c>
       <c r="D137" s="5">
@@ -27657,7 +28503,8 @@
       <c r="B138">
         <v>10</v>
       </c>
-      <c r="C138">
+      <c r="C138" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A138,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C138),2)</f>
         <v>-10</v>
       </c>
       <c r="D138" s="5">
@@ -27708,7 +28555,8 @@
       <c r="B139">
         <v>20</v>
       </c>
-      <c r="C139">
+      <c r="C139" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A139,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C139),2)</f>
         <v>-20</v>
       </c>
       <c r="D139" s="5">
@@ -27759,7 +28607,8 @@
       <c r="B140">
         <v>40</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A140,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C140),2)</f>
         <v>-40</v>
       </c>
       <c r="D140" s="5">
@@ -27810,7 +28659,8 @@
       <c r="B141">
         <v>2.5</v>
       </c>
-      <c r="C141">
+      <c r="C141" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A141,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C141),2)</f>
         <v>-2.5</v>
       </c>
       <c r="D141" s="5">
@@ -27861,7 +28711,8 @@
       <c r="B142">
         <v>5</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A142,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C142),2)</f>
         <v>-5</v>
       </c>
       <c r="D142" s="5">
@@ -27912,7 +28763,8 @@
       <c r="B143">
         <v>10</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A143,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C143),2)</f>
         <v>-10</v>
       </c>
       <c r="D143" s="5">
@@ -27963,7 +28815,8 @@
       <c r="B144">
         <v>5</v>
       </c>
-      <c r="C144">
+      <c r="C144" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A144,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C144),2)</f>
         <v>-5</v>
       </c>
       <c r="D144" s="5">
@@ -28014,7 +28867,8 @@
       <c r="B145">
         <v>10</v>
       </c>
-      <c r="C145">
+      <c r="C145" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A145,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C145),2)</f>
         <v>-10</v>
       </c>
       <c r="D145" s="5">
@@ -28065,7 +28919,8 @@
       <c r="B146">
         <v>20</v>
       </c>
-      <c r="C146">
+      <c r="C146" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A146,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C146),2)</f>
         <v>-20</v>
       </c>
       <c r="D146" s="5">
@@ -28116,7 +28971,8 @@
       <c r="B147">
         <v>7.5</v>
       </c>
-      <c r="C147">
+      <c r="C147" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A147,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C147),2)</f>
         <v>-7.5</v>
       </c>
       <c r="D147" s="5">
@@ -28167,7 +29023,8 @@
       <c r="B148">
         <v>15</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A148,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C148),2)</f>
         <v>-15</v>
       </c>
       <c r="D148" s="5">
@@ -28218,7 +29075,8 @@
       <c r="B149">
         <v>30</v>
       </c>
-      <c r="C149">
+      <c r="C149" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A149,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C149),2)</f>
         <v>-30</v>
       </c>
       <c r="D149" s="5">
@@ -28269,7 +29127,8 @@
       <c r="B150">
         <v>10</v>
       </c>
-      <c r="C150">
+      <c r="C150" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A150,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C150),2)</f>
         <v>-10</v>
       </c>
       <c r="D150" s="5">
@@ -28320,7 +29179,8 @@
       <c r="B151">
         <v>20</v>
       </c>
-      <c r="C151">
+      <c r="C151" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A151,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C151),2)</f>
         <v>-20</v>
       </c>
       <c r="D151" s="5">
@@ -28371,7 +29231,8 @@
       <c r="B152">
         <v>40</v>
       </c>
-      <c r="C152">
+      <c r="C152" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A152,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C152),2)</f>
         <v>-40</v>
       </c>
       <c r="D152" s="5">
@@ -28419,6 +29280,7 @@
       <c r="A153" s="15" t="s">
         <v>189</v>
       </c>
+      <c r="C153" s="5"/>
       <c r="D153" s="5"/>
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
@@ -28434,7 +29296,8 @@
       <c r="B154">
         <v>15</v>
       </c>
-      <c r="C154">
+      <c r="C154" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A154,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C154),2)</f>
         <v>-15</v>
       </c>
       <c r="D154" s="5">
@@ -28485,7 +29348,8 @@
       <c r="B155">
         <v>5</v>
       </c>
-      <c r="C155">
+      <c r="C155" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A155,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C155),2)</f>
         <v>-5</v>
       </c>
       <c r="D155" s="5">
@@ -28536,7 +29400,8 @@
       <c r="B156">
         <v>10</v>
       </c>
-      <c r="C156">
+      <c r="C156" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A156,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C156),2)</f>
         <v>-10</v>
       </c>
       <c r="D156" s="5">
@@ -28587,7 +29452,8 @@
       <c r="B157">
         <v>20</v>
       </c>
-      <c r="C157">
+      <c r="C157" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A157,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C157),2)</f>
         <v>-20</v>
       </c>
       <c r="D157" s="5">
@@ -28638,7 +29504,8 @@
       <c r="B158">
         <v>7.5</v>
       </c>
-      <c r="C158">
+      <c r="C158" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A158,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C158),2)</f>
         <v>-7.5</v>
       </c>
       <c r="D158" s="5">
@@ -28689,7 +29556,8 @@
       <c r="B159">
         <v>15</v>
       </c>
-      <c r="C159">
+      <c r="C159" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A159,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C159),2)</f>
         <v>-15</v>
       </c>
       <c r="D159" s="5">
@@ -28740,7 +29608,8 @@
       <c r="B160">
         <v>7.5</v>
       </c>
-      <c r="C160">
+      <c r="C160" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A160,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C160),2)</f>
         <v>-7.5</v>
       </c>
       <c r="D160" s="5">
@@ -28791,7 +29660,8 @@
       <c r="B161">
         <v>15</v>
       </c>
-      <c r="C161">
+      <c r="C161" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A161,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C161),2)</f>
         <v>-15</v>
       </c>
       <c r="D161" s="5">
@@ -28839,6 +29709,7 @@
       <c r="A162" s="15" t="s">
         <v>198</v>
       </c>
+      <c r="C162" s="5"/>
       <c r="D162" s="5"/>
       <c r="E162" s="5"/>
       <c r="F162" s="5"/>
@@ -28854,7 +29725,8 @@
       <c r="B163">
         <v>15</v>
       </c>
-      <c r="C163">
+      <c r="C163" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A163,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C163),2)</f>
         <v>-15</v>
       </c>
       <c r="D163" s="5">
@@ -28905,7 +29777,8 @@
       <c r="B164">
         <v>30</v>
       </c>
-      <c r="C164">
+      <c r="C164" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A164,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C164),2)</f>
         <v>-30</v>
       </c>
       <c r="D164" s="5">
@@ -28956,7 +29829,8 @@
       <c r="B165">
         <v>60</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A165,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C165),2)</f>
         <v>-60</v>
       </c>
       <c r="D165" s="5">
@@ -29004,6 +29878,7 @@
       <c r="A166" s="15" t="s">
         <v>202</v>
       </c>
+      <c r="C166" s="5"/>
       <c r="D166" s="5"/>
       <c r="E166" s="5"/>
       <c r="F166" s="5"/>
@@ -29019,7 +29894,8 @@
       <c r="B167">
         <v>0</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A167,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C167),2)</f>
         <v>0</v>
       </c>
       <c r="D167" s="5">
@@ -29070,7 +29946,8 @@
       <c r="B168">
         <v>0</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A168,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C168),2)</f>
         <v>0</v>
       </c>
       <c r="D168" s="5">
@@ -29121,7 +29998,8 @@
       <c r="B169">
         <v>0</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A169,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C169),2)</f>
         <v>0</v>
       </c>
       <c r="D169" s="5">
@@ -29172,7 +30050,8 @@
       <c r="B170">
         <v>50</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A170,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C170),2)</f>
         <v>-50</v>
       </c>
       <c r="D170" s="5">
@@ -29223,7 +30102,8 @@
       <c r="B171">
         <v>12.5</v>
       </c>
-      <c r="C171">
+      <c r="C171" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A171,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C171),2)</f>
         <v>-12.5</v>
       </c>
       <c r="D171" s="5">
@@ -29274,7 +30154,8 @@
       <c r="B172">
         <v>25</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A172,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C172),2)</f>
         <v>-25</v>
       </c>
       <c r="D172" s="5">
@@ -29322,6 +30203,7 @@
       <c r="A173" s="15" t="s">
         <v>209</v>
       </c>
+      <c r="C173" s="5"/>
       <c r="D173" s="5"/>
       <c r="E173" s="5"/>
       <c r="F173" s="5"/>
@@ -29337,7 +30219,8 @@
       <c r="B174">
         <v>0</v>
       </c>
-      <c r="C174">
+      <c r="C174" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A174,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C174),2)</f>
         <v>0</v>
       </c>
       <c r="D174" s="5">
@@ -29385,6 +30268,7 @@
       <c r="A175" s="15" t="s">
         <v>211</v>
       </c>
+      <c r="C175" s="5"/>
       <c r="D175" s="5"/>
       <c r="E175" s="5"/>
       <c r="F175" s="5"/>
@@ -29400,7 +30284,8 @@
       <c r="B176">
         <v>5</v>
       </c>
-      <c r="C176">
+      <c r="C176" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A176,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C176),2)</f>
         <v>-5</v>
       </c>
       <c r="D176" s="5">
@@ -29450,7 +30335,8 @@
       <c r="B177">
         <v>7.5</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A177,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C177),2)</f>
         <v>-7.5</v>
       </c>
       <c r="D177" s="5">
@@ -29500,7 +30386,8 @@
       <c r="B178">
         <v>10</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="5">
+        <f>ROUND(_xlfn.IFNA(VLOOKUP(A178,'Weapon Formulas'!$E$10:$V$115,17,0),weapon_components!C178),2)</f>
         <v>-10</v>
       </c>
       <c r="D178" s="5">

</xml_diff>

<commit_message>
auras costed to 25% of max battleship power
</commit_message>
<xml_diff>
--- a/Stellaris Rebalance.xlsx
+++ b/Stellaris Rebalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="737" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="737" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="weapon_components" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="262">
   <si>
     <t># Lines starting with ”#” will be treated as comments.</t>
   </si>
@@ -805,6 +805,9 @@
   </si>
   <si>
     <t>Power</t>
+  </si>
+  <si>
+    <t>Auras Cost</t>
   </si>
 </sst>
 </file>
@@ -21645,10 +21648,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21800,6 +21803,15 @@
         <v>53.333333333333329</v>
       </c>
     </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>261</v>
+      </c>
+      <c r="J10">
+        <f>64*0.25*J6</f>
+        <v>1280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21810,7 +21822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
armor and manv per tier gain updated, armor costs power
</commit_message>
<xml_diff>
--- a/Stellaris Rebalance.xlsx
+++ b/Stellaris Rebalance.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="275">
   <si>
     <t># Lines starting with ”#” will be treated as comments.</t>
   </si>
@@ -807,17 +807,57 @@
     <t>Power</t>
   </si>
   <si>
-    <t>Auras Cost</t>
+    <t>Slots Left</t>
+  </si>
+  <si>
+    <t>Max Defense per tier</t>
+  </si>
+  <si>
+    <t>Shields</t>
+  </si>
+  <si>
+    <t>Evasion Mult</t>
+  </si>
+  <si>
+    <t>Armor Add</t>
+  </si>
+  <si>
+    <t>Per Slot</t>
+  </si>
+  <si>
+    <t>True Max Evasion</t>
+  </si>
+  <si>
+    <t>Normal Max Armor</t>
+  </si>
+  <si>
+    <t>Total Evasion</t>
+  </si>
+  <si>
+    <t>Total Armor Needed</t>
+  </si>
+  <si>
+    <t>Max Possible Armor</t>
+  </si>
+  <si>
+    <t>Max Possible Armor %</t>
+  </si>
+  <si>
+    <t>Normal Shield HP %</t>
+  </si>
+  <si>
+    <t>HP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
     <numFmt numFmtId="165" formatCode="#"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -894,7 +934,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -918,6 +958,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12215,8 +12257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP121"/>
   <sheetViews>
-    <sheetView topLeftCell="L94" workbookViewId="0">
-      <selection activeCell="W104" sqref="W104"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12605,11 +12647,11 @@
       <c r="F8" s="12">
         <v>0.2</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="W8">
@@ -21648,10 +21690,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21662,7 +21704,7 @@
     <col min="4" max="4" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>250</v>
       </c>
@@ -21684,8 +21726,11 @@
       <c r="K1" s="14" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
@@ -21714,8 +21759,17 @@
         <f>2/3*J2</f>
         <v>3.333333333333333</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>263</v>
+      </c>
+      <c r="P2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>256</v>
       </c>
@@ -21742,8 +21796,21 @@
         <f t="shared" ref="K3:K6" si="0">2/3*J3</f>
         <v>6.6666666666666661</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O3" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P3" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S3">
+        <f>80/5</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>257</v>
       </c>
@@ -21774,10 +21841,39 @@
         <f t="shared" si="0"/>
         <v>13.333333333333332</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="M4" t="s">
+        <v>266</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="P4" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5">
+        <f>B3-B4</f>
+        <v>6</v>
+      </c>
+      <c r="C5" s="23">
+        <f t="shared" ref="C5:E5" si="3">C3-C4</f>
+        <v>12</v>
+      </c>
+      <c r="D5" s="23">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
       <c r="I5">
         <v>4</v>
       </c>
@@ -21789,8 +21885,36 @@
         <f t="shared" si="0"/>
         <v>26.666666666666664</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N5" s="24">
+        <f>N3/$B5</f>
+        <v>2.3333333333333334E-2</v>
+      </c>
+      <c r="O5" s="12">
+        <v>40</v>
+      </c>
+      <c r="P5" s="12">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+      <c r="C6">
+        <f>B6*2</f>
+        <v>600</v>
+      </c>
+      <c r="D6" s="23">
+        <f t="shared" ref="D6:E6" si="4">C6*2</f>
+        <v>1200</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="4"/>
+        <v>2400</v>
+      </c>
       <c r="I6">
         <v>5</v>
       </c>
@@ -21803,13 +21927,322 @@
         <v>53.333333333333329</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H10" t="s">
-        <v>261</v>
-      </c>
-      <c r="J10">
-        <f>64*0.25*J6</f>
-        <v>1280</v>
+    <row r="7" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="23">
+        <v>1</v>
+      </c>
+      <c r="C7" s="23">
+        <f>(C11/C8)-1</f>
+        <v>-0.625</v>
+      </c>
+      <c r="D7" s="23">
+        <f t="shared" ref="D7:E7" si="5">(D11/D8)-1</f>
+        <v>-0.875</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" si="5"/>
+        <v>-0.96875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="23">
+        <f>B3*$N$5</f>
+        <v>0.18666666666666668</v>
+      </c>
+      <c r="C8" s="23">
+        <f>C3*$N$5</f>
+        <v>0.37333333333333335</v>
+      </c>
+      <c r="D8" s="23">
+        <f>D3*$N$5</f>
+        <v>0.7466666666666667</v>
+      </c>
+      <c r="E8" s="23">
+        <f>E3*$N$5</f>
+        <v>1.4933333333333334</v>
+      </c>
+      <c r="O8" s="23">
+        <f>O5/5</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9" s="23">
+        <f t="shared" ref="B9:D9" si="6">(B13-B14)</f>
+        <v>0.11963190184049211</v>
+      </c>
+      <c r="C9" s="23">
+        <f t="shared" si="6"/>
+        <v>8.2380952380952337</v>
+      </c>
+      <c r="D9" s="23">
+        <f t="shared" si="6"/>
+        <v>20.831460674157285</v>
+      </c>
+      <c r="E9" s="23">
+        <f>(E13-E14)</f>
+        <v>62.769230769230745</v>
+      </c>
+      <c r="P9">
+        <f>P5/5</f>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="I10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B11" s="24">
+        <f>B3*$N$5*B7</f>
+        <v>0.18666666666666668</v>
+      </c>
+      <c r="C11" s="24">
+        <f>B11*(3/4)</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D11" s="24">
+        <f>B11*(2/4)</f>
+        <v>9.3333333333333338E-2</v>
+      </c>
+      <c r="E11" s="24">
+        <f>B11/4</f>
+        <v>4.6666666666666669E-2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>130</v>
+      </c>
+      <c r="J11">
+        <f>B3</f>
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>12</v>
+      </c>
+      <c r="L11">
+        <v>24</v>
+      </c>
+      <c r="M11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.185</v>
+      </c>
+      <c r="C12" s="10">
+        <f>B12*2</f>
+        <v>0.37</v>
+      </c>
+      <c r="D12" s="10">
+        <f>B12*3</f>
+        <v>0.55499999999999994</v>
+      </c>
+      <c r="E12" s="10">
+        <f>B12*4</f>
+        <v>0.74</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="10">
+        <f>(($P$5*$I12)*J$11)/((($P$5*$I12)*J$11)+60)</f>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="K12" s="10">
+        <f t="shared" ref="K12:M16" si="7">(($P$5*$I12)*K$11)/((($P$5*$I12)*K$11)+60)</f>
+        <v>0.31034482758620691</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" si="7"/>
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="M12" s="10">
+        <f t="shared" si="7"/>
+        <v>0.6428571428571429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="B13" s="23">
+        <f>-((60*B12)/(B12-1))</f>
+        <v>13.619631901840492</v>
+      </c>
+      <c r="C13" s="23">
+        <f t="shared" ref="B13:D13" si="8">-((60*C12)/(C12-1))</f>
+        <v>35.238095238095234</v>
+      </c>
+      <c r="D13" s="23">
+        <f t="shared" si="8"/>
+        <v>74.831460674157285</v>
+      </c>
+      <c r="E13" s="23">
+        <f>-((60*E12)/(E12-1))</f>
+        <v>170.76923076923075</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13" s="10">
+        <f t="shared" ref="J13:J16" si="9">(($P$5*$I13)*J$11)/((($P$5*$I13)*J$11)+60)</f>
+        <v>0.375</v>
+      </c>
+      <c r="K13" s="10">
+        <f t="shared" si="7"/>
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="L13" s="10">
+        <f t="shared" si="7"/>
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="M13" s="10">
+        <f t="shared" si="7"/>
+        <v>0.78260869565217395</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="B14" s="23">
+        <f>$P$5*B5</f>
+        <v>13.5</v>
+      </c>
+      <c r="C14" s="23">
+        <f>$P$5*C5</f>
+        <v>27</v>
+      </c>
+      <c r="D14" s="23">
+        <f>$P$5*D5</f>
+        <v>54</v>
+      </c>
+      <c r="E14" s="23">
+        <f>$P$5*E5</f>
+        <v>108</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14" s="10">
+        <f t="shared" si="9"/>
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="K14" s="10">
+        <f t="shared" si="7"/>
+        <v>0.57446808510638303</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="7"/>
+        <v>0.72972972972972971</v>
+      </c>
+      <c r="M14" s="10">
+        <f t="shared" si="7"/>
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B15" s="10">
+        <f>((B3*$P$5)+B9)/((B3*$P$5)+60+B9)</f>
+        <v>0.23194722582165156</v>
+      </c>
+      <c r="C15" s="10">
+        <f>((C3*$P$5)+C9)/((C3*$P$5)+60+C9)</f>
+        <v>0.42439470077661029</v>
+      </c>
+      <c r="D15" s="10">
+        <f>((D3*$P$5)+D9)/((D3*$P$5)+60+D9)</f>
+        <v>0.60741067490074985</v>
+      </c>
+      <c r="E15" s="10">
+        <f>((E3*$P$5)+E9)/((E3*$P$5)+60+E9)</f>
+        <v>0.77508650519031153</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15" s="10">
+        <f t="shared" si="9"/>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="K15" s="10">
+        <f t="shared" si="7"/>
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="7"/>
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="M15" s="10">
+        <f t="shared" si="7"/>
+        <v>0.87804878048780488</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16">
+        <f>(B5*$O$5)/B6</f>
+        <v>0.8</v>
+      </c>
+      <c r="C16" s="23">
+        <f t="shared" ref="C16:E16" si="10">(C5*$O$5)/C6</f>
+        <v>0.8</v>
+      </c>
+      <c r="D16" s="23">
+        <f t="shared" si="10"/>
+        <v>0.8</v>
+      </c>
+      <c r="E16" s="23">
+        <f t="shared" si="10"/>
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="23"/>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16" s="10">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="K16" s="10">
+        <f t="shared" si="7"/>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="7"/>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="M16" s="10">
+        <f t="shared" si="7"/>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -21822,7 +22255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U179"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -21925,7 +22358,7 @@
         <v>146</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="24"/>
+      <c r="P4" s="26"/>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -21954,7 +22387,7 @@
         <v>147</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="25"/>
+      <c r="P5" s="27"/>
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -22003,7 +22436,7 @@
       <c r="O6" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="P6" s="25"/>
+      <c r="P6" s="27"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -22024,7 +22457,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="25"/>
+      <c r="P7" s="27"/>
       <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed unknown armor error, changed Z offset
</commit_message>
<xml_diff>
--- a/Stellaris Rebalance.xlsx
+++ b/Stellaris Rebalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="737" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="737" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="weapon_components" sheetId="4" r:id="rId1"/>
@@ -12927,7 +12927,7 @@
         <v>0.8</v>
       </c>
       <c r="S12" s="25">
-        <f t="shared" ref="S12:S27" si="14">($S$9)*(1+(D12*$F$8))*(1+((C12-1)*$J$3))</f>
+        <f t="shared" ref="S12:S25" si="14">($S$9)*(1+(D12*$F$8))*(1+((C12-1)*$J$3))</f>
         <v>30</v>
       </c>
       <c r="T12" s="2">
@@ -14418,7 +14418,7 @@
         <v>247</v>
       </c>
       <c r="S29" s="2">
-        <f t="shared" ref="S12:S29" si="21">$S$9*(1+(D29*$F$8))</f>
+        <f t="shared" ref="S29" si="21">$S$9*(1+(D29*$F$8))</f>
         <v>30</v>
       </c>
       <c r="T29" s="2">
@@ -14727,7 +14727,7 @@
         <v>0.8</v>
       </c>
       <c r="S31" s="25">
-        <f t="shared" ref="S31:S40" si="32">($S$29)*(1+(D31*$F$8))*(1+((C31-1)*$J$3))</f>
+        <f t="shared" ref="S31:S38" si="32">($S$29)*(1+(D31*$F$8))*(1+((C31-1)*$J$3))</f>
         <v>37.200000000000003</v>
       </c>
       <c r="T31" s="2">
@@ -16221,7 +16221,7 @@
         <v>0.8</v>
       </c>
       <c r="S44" s="25">
-        <f t="shared" ref="S44:S53" si="46">($S$42)*(1+(D44*$F$8))*(1+((C44-1)*$J$3))</f>
+        <f t="shared" ref="S44:S51" si="46">($S$42)*(1+(D44*$F$8))*(1+((C44-1)*$J$3))</f>
         <v>26.04</v>
       </c>
       <c r="T44" s="2">
@@ -17160,7 +17160,7 @@
         <v>0.72</v>
       </c>
       <c r="S57" s="25">
-        <f t="shared" ref="S57:S72" si="57">($S$55)*(1+(D57*$F$8))*(1+((C57-1)*$J$3))</f>
+        <f t="shared" ref="S57:S69" si="57">($S$55)*(1+(D57*$F$8))*(1+((C57-1)*$J$3))</f>
         <v>45</v>
       </c>
       <c r="T57" s="2">
@@ -19438,7 +19438,7 @@
         <v>1</v>
       </c>
       <c r="S89" s="25">
-        <f t="shared" ref="S89:S104" si="72">($S$87)*(1+(D89*$F$8))*(1+((C89-1)*$J$3))</f>
+        <f t="shared" ref="S89:S102" si="72">($S$87)*(1+(D89*$F$8))*(1+((C89-1)*$J$3))</f>
         <v>60</v>
       </c>
       <c r="T89" s="2">
@@ -20634,7 +20634,7 @@
         <v>1</v>
       </c>
       <c r="S105" s="25">
-        <f t="shared" ref="S105:S114" si="82">($S$103)*(1+(D105*$F$8))*(1+((C105-1)*$J$3))</f>
+        <f t="shared" ref="S105:S112" si="82">($S$103)*(1+(D105*$F$8))*(1+((C105-1)*$J$3))</f>
         <v>74.400000000000006</v>
       </c>
       <c r="T105" s="2">
@@ -21700,8 +21700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22263,7 +22263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+    <sheetView topLeftCell="A138" workbookViewId="0">
       <selection activeCell="W139" sqref="W139"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed error with no closing ;
</commit_message>
<xml_diff>
--- a/Stellaris Rebalance.xlsx
+++ b/Stellaris Rebalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="737" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="737" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="weapon_components" sheetId="4" r:id="rId1"/>
@@ -1065,6 +1065,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1072,7 +1073,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20559,11 +20559,11 @@
       <c r="F8" s="12">
         <v>0.2</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="W8">
@@ -20795,7 +20795,7 @@
         <v>2.67225</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" ref="I11:J25" si="9">$F12*(INDEX($F$3:$F$5,I$9)+(($C12+($D12*$F$7))*INDEX($G$3:$G$5,I$9)))</f>
+        <f t="shared" ref="I12:J25" si="9">$F12*(INDEX($F$3:$F$5,I$9)+(($C12+($D12*$F$7))*INDEX($G$3:$G$5,I$9)))</f>
         <v>1.8323999999999998</v>
       </c>
       <c r="J12" s="2">
@@ -26684,7 +26684,7 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="K77" s="10">
-        <f t="shared" ref="K77:K124" ca="1" si="66">1-((1-(I77/(G77*R77)))/INDEX($P$2:$P$6,C77))</f>
+        <f t="shared" ref="K77:K122" ca="1" si="66">1-((1-(I77/(G77*R77)))/INDEX($P$2:$P$6,C77))</f>
         <v>3.7027155255156874</v>
       </c>
       <c r="L77" s="10">
@@ -30242,7 +30242,7 @@
         <v>8.7880441322300094</v>
       </c>
       <c r="L125" s="10">
-        <f t="shared" ref="L125:L149" si="94">(INDEX($Q$2:$Q$6,C125)/((1/INDEX($F$4:$F$6,J$123))-1))</f>
+        <f t="shared" ref="L125:L147" si="94">(INDEX($Q$2:$Q$6,C125)/((1/INDEX($F$4:$F$6,J$123))-1))</f>
         <v>8.8888888888888889E-3</v>
       </c>
       <c r="M125" s="10">
@@ -33817,7 +33817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -34208,19 +34208,19 @@
         <v>1</v>
       </c>
       <c r="J12" s="10">
-        <f>($P$6*$I12*B$5*B$11)/(($P$6*$I12*B$5*B$11)+60)</f>
+        <f t="shared" ref="J12:M16" si="8">($P$6*$I12*B$5*B$11)/(($P$6*$I12*B$5*B$11)+60)</f>
         <v>4.4117647058823539E-2</v>
       </c>
       <c r="K12" s="10">
-        <f>($P$6*$I12*C$5*C$11)/(($P$6*$I12*C$5*C$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.10714285714285714</v>
       </c>
       <c r="L12" s="10">
-        <f>($P$6*$I12*D$5*D$11)/(($P$6*$I12*D$5*D$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="M12" s="10">
-        <f>($P$6*$I12*E$5*E$11)/(($P$6*$I12*E$5*E$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.37500000000000006</v>
       </c>
     </row>
@@ -34233,11 +34233,11 @@
         <v>13.846153846153847</v>
       </c>
       <c r="C13" s="27">
-        <f t="shared" ref="C13:D13" si="8">-(60*C12)/(C12-1)</f>
+        <f t="shared" ref="C13:D13" si="9">-(60*C12)/(C12-1)</f>
         <v>36</v>
       </c>
       <c r="D13" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>77.142857142857139</v>
       </c>
       <c r="E13" s="27">
@@ -34248,19 +34248,19 @@
         <v>2</v>
       </c>
       <c r="J13" s="10">
-        <f>($P$6*$I13*B$5*B$11)/(($P$6*$I13*B$5*B$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>8.4507042253521139E-2</v>
       </c>
       <c r="K13" s="10">
-        <f>($P$6*$I13*C$5*C$11)/(($P$6*$I13*C$5*C$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.19354838709677419</v>
       </c>
       <c r="L13" s="10">
-        <f>($P$6*$I13*D$5*D$11)/(($P$6*$I13*D$5*D$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.339622641509434</v>
       </c>
       <c r="M13" s="10">
-        <f>($P$6*$I13*E$5*E$11)/(($P$6*$I13*E$5*E$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.54545454545454553</v>
       </c>
     </row>
@@ -34289,19 +34289,19 @@
         <v>3</v>
       </c>
       <c r="J14" s="10">
-        <f>($P$6*$I14*B$5*B$11)/(($P$6*$I14*B$5*B$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.12162162162162166</v>
       </c>
       <c r="K14" s="10">
-        <f>($P$6*$I14*C$5*C$11)/(($P$6*$I14*C$5*C$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.26470588235294124</v>
       </c>
       <c r="L14" s="10">
-        <f>($P$6*$I14*D$5*D$11)/(($P$6*$I14*D$5*D$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.43548387096774199</v>
       </c>
       <c r="M14" s="10">
-        <f>($P$6*$I14*E$5*E$11)/(($P$6*$I14*E$5*E$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.6428571428571429</v>
       </c>
     </row>
@@ -34314,11 +34314,11 @@
         <v>13.846153846153847</v>
       </c>
       <c r="C15" s="27">
-        <f t="shared" ref="C15:E15" si="9">-(60*(C12))/((C12)-1)</f>
+        <f t="shared" ref="C15:D15" si="10">-(60*(C12))/((C12)-1)</f>
         <v>36</v>
       </c>
       <c r="D15" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>77.142857142857139</v>
       </c>
       <c r="E15" s="27">
@@ -34329,19 +34329,19 @@
         <v>4</v>
       </c>
       <c r="J15" s="10">
-        <f>($P$6*$I15*B$5*B$11)/(($P$6*$I15*B$5*B$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.15584415584415587</v>
       </c>
       <c r="K15" s="10">
-        <f>($P$6*$I15*C$5*C$11)/(($P$6*$I15*C$5*C$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.32432432432432434</v>
       </c>
       <c r="L15" s="10">
-        <f>($P$6*$I15*D$5*D$11)/(($P$6*$I15*D$5*D$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.50704225352112675</v>
       </c>
       <c r="M15" s="10">
-        <f>($P$6*$I15*E$5*E$11)/(($P$6*$I15*E$5*E$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.70588235294117652</v>
       </c>
     </row>
@@ -34360,19 +34360,19 @@
         <v>5</v>
       </c>
       <c r="J16" s="10">
-        <f>($P$6*$I16*B$5*B$11)/(($P$6*$I16*B$5*B$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.1875</v>
       </c>
       <c r="K16" s="10">
-        <f>($P$6*$I16*C$5*C$11)/(($P$6*$I16*C$5*C$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.375</v>
       </c>
       <c r="L16" s="10">
-        <f>($P$6*$I16*D$5*D$11)/(($P$6*$I16*D$5*D$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.5625</v>
       </c>
       <c r="M16" s="10">
-        <f>($P$6*$I16*E$5*E$11)/(($P$6*$I16*E$5*E$11)+60)</f>
+        <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
     </row>
@@ -34421,7 +34421,7 @@
         <f ca="1">G6</f>
         <v>0.86852188974575439</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="35">
         <f ca="1">B9</f>
         <v>0.7</v>
       </c>
@@ -34437,11 +34437,11 @@
         <v>0.16119340416507255</v>
       </c>
       <c r="K19" s="10">
-        <f t="shared" ref="K19:L23" ca="1" si="10">1-(($G$6-($I19*$N$5*C$5*C$7))/$G$6)</f>
+        <f t="shared" ref="K19:L23" ca="1" si="11">1-(($G$6-($I19*$N$5*C$5*C$7))/$G$6)</f>
         <v>0.1197436716654825</v>
       </c>
       <c r="L19" s="10">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>8.059670208253622E-2</v>
       </c>
       <c r="M19" s="10">
@@ -34472,19 +34472,19 @@
         <v>2</v>
       </c>
       <c r="J20" s="10">
-        <f t="shared" ref="J20:J22" ca="1" si="11">1-(($G$6-($N$5*B$5*$I20*(B$7)))/$G$6)</f>
+        <f t="shared" ref="J20:J22" ca="1" si="12">1-(($G$6-($N$5*B$5*$I20*(B$7)))/$G$6)</f>
         <v>0.3223868083301451</v>
       </c>
       <c r="K20" s="10">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0.239487343330965</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0.16119340416507255</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" ref="M20:M22" ca="1" si="12">1-(($G$6-($I20*$N$5*E$5*E$7))/$G$6)</f>
+        <f t="shared" ref="M20:M22" ca="1" si="13">1-(($G$6-($I20*$N$5*E$5*E$7))/$G$6)</f>
         <v>7.8293939165892334E-2</v>
       </c>
     </row>
@@ -34493,19 +34493,19 @@
         <v>3</v>
       </c>
       <c r="J21" s="10">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.48358021249521765</v>
+      </c>
+      <c r="K21" s="10">
         <f t="shared" ca="1" si="11"/>
-        <v>0.48358021249521765</v>
-      </c>
-      <c r="K21" s="10">
-        <f t="shared" ca="1" si="10"/>
         <v>0.35923101499644738</v>
       </c>
       <c r="L21" s="10">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0.24179010624760888</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0.11744090874883861</v>
       </c>
     </row>
@@ -34514,19 +34514,19 @@
         <v>4</v>
       </c>
       <c r="J22" s="10">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.64477361666029021</v>
+      </c>
+      <c r="K22" s="10">
         <f t="shared" ca="1" si="11"/>
-        <v>0.64477361666029021</v>
-      </c>
-      <c r="K22" s="10">
-        <f t="shared" ca="1" si="10"/>
         <v>0.47897468666192999</v>
       </c>
       <c r="L22" s="10">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0.3223868083301451</v>
       </c>
       <c r="M22" s="10">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0.15658787833178478</v>
       </c>
     </row>
@@ -34539,11 +34539,11 @@
         <v>0.80596702082536287</v>
       </c>
       <c r="K23" s="10">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0.59871835832741249</v>
       </c>
       <c r="L23" s="10">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0.40298351041268143</v>
       </c>
       <c r="M23" s="10">
@@ -34564,7 +34564,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E28" s="10">
-        <f ca="1">1-($G$6-(F28/100))/$G$6</f>
+        <f t="shared" ref="E28:E59" ca="1" si="14">1-($G$6-(F28/100))/$G$6</f>
         <v>1.1513814583219428E-2</v>
       </c>
       <c r="F28">
@@ -34577,3186 +34577,3186 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E29" s="10">
-        <f ca="1">1-($G$6-(F29/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>2.3027629166438968E-2</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
       <c r="G29" s="10">
-        <f t="shared" ref="G29:G92" si="13">F29/(F29+60)</f>
+        <f t="shared" ref="G29:G92" si="15">F29/(F29+60)</f>
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E30" s="10">
-        <f ca="1">1-($G$6-(F30/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>3.4541443749658396E-2</v>
       </c>
       <c r="F30">
         <v>3</v>
       </c>
       <c r="G30" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.7619047619047616E-2</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E31" s="10">
-        <f ca="1">1-($G$6-(F31/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>4.6055258332877935E-2</v>
       </c>
       <c r="F31">
         <v>4</v>
       </c>
       <c r="G31" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E32" s="10">
-        <f ca="1">1-($G$6-(F32/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>5.7569072916097364E-2</v>
       </c>
       <c r="F32">
         <v>5</v>
       </c>
       <c r="G32" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" s="10">
-        <f ca="1">1-($G$6-(F33/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>6.9082887499316792E-2</v>
       </c>
       <c r="F33">
         <v>6</v>
       </c>
       <c r="G33" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34" s="10">
-        <f ca="1">1-($G$6-(F34/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>8.059670208253622E-2</v>
       </c>
       <c r="F34">
         <v>7</v>
       </c>
       <c r="G34" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.1044776119402985</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35" s="10">
-        <f ca="1">1-($G$6-(F35/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>9.2110516665755759E-2</v>
       </c>
       <c r="F35">
         <v>8</v>
       </c>
       <c r="G35" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.11764705882352941</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36" s="10">
-        <f ca="1">1-($G$6-(F36/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.10362433124897519</v>
       </c>
       <c r="F36">
         <v>9</v>
       </c>
       <c r="G36" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.13043478260869565</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E37" s="10">
-        <f ca="1">1-($G$6-(F37/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.11513814583219473</v>
       </c>
       <c r="F37">
         <v>10</v>
       </c>
       <c r="G37" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E38" s="10">
-        <f ca="1">1-($G$6-(F38/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.12665196041541416</v>
       </c>
       <c r="F38" s="33">
         <v>11</v>
       </c>
       <c r="G38" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.15492957746478872</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E39" s="10">
-        <f ca="1">1-($G$6-(F39/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.13816577499863369</v>
       </c>
       <c r="F39" s="33">
         <v>12</v>
       </c>
       <c r="G39" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="40" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E40" s="10">
-        <f ca="1">1-($G$6-(F40/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.14967958958185312</v>
       </c>
       <c r="F40" s="33">
         <v>13</v>
       </c>
       <c r="G40" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.17808219178082191</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E41" s="10">
-        <f ca="1">1-($G$6-(F41/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.16119340416507255</v>
       </c>
       <c r="F41" s="33">
         <v>14</v>
       </c>
       <c r="G41" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.1891891891891892</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E42" s="10">
-        <f ca="1">1-($G$6-(F42/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.17270721874829209</v>
       </c>
       <c r="F42" s="33">
         <v>15</v>
       </c>
       <c r="G42" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E43" s="10">
-        <f ca="1">1-($G$6-(F43/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.18422103333151152</v>
       </c>
       <c r="F43" s="33">
         <v>16</v>
       </c>
       <c r="G43" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.21052631578947367</v>
       </c>
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E44" s="10">
-        <f ca="1">1-($G$6-(F44/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.19573484791473106</v>
       </c>
       <c r="F44" s="33">
         <v>17</v>
       </c>
       <c r="G44" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.22077922077922077</v>
       </c>
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E45" s="10">
-        <f ca="1">1-($G$6-(F45/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.20724866249795049</v>
       </c>
       <c r="F45" s="33">
         <v>18</v>
       </c>
       <c r="G45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.23076923076923078</v>
       </c>
     </row>
     <row r="46" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E46" s="10">
-        <f ca="1">1-($G$6-(F46/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.21876247708117003</v>
       </c>
       <c r="F46" s="33">
         <v>19</v>
       </c>
       <c r="G46" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.24050632911392406</v>
       </c>
     </row>
     <row r="47" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E47" s="10">
-        <f ca="1">1-($G$6-(F47/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.23027629166438945</v>
       </c>
       <c r="F47" s="33">
         <v>20</v>
       </c>
       <c r="G47" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="48" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E48" s="10">
-        <f ca="1">1-($G$6-(F48/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.24179010624760888</v>
       </c>
       <c r="F48" s="33">
         <v>21</v>
       </c>
       <c r="G48" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.25925925925925924</v>
       </c>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E49" s="10">
-        <f ca="1">1-($G$6-(F49/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.25330392083082831</v>
       </c>
       <c r="F49" s="33">
         <v>22</v>
       </c>
       <c r="G49" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.26829268292682928</v>
       </c>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E50" s="10">
-        <f ca="1">1-($G$6-(F50/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.26481773541404785</v>
       </c>
       <c r="F50" s="33">
         <v>23</v>
       </c>
       <c r="G50" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.27710843373493976</v>
       </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E51" s="10">
-        <f ca="1">1-($G$6-(F51/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.27633154999726728</v>
       </c>
       <c r="F51" s="33">
         <v>24</v>
       </c>
       <c r="G51" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52" s="10">
-        <f ca="1">1-($G$6-(F52/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.28784536458048671</v>
       </c>
       <c r="F52" s="33">
         <v>25</v>
       </c>
       <c r="G52" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.29411764705882354</v>
       </c>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53" s="10">
-        <f ca="1">1-($G$6-(F53/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.29935917916370625</v>
       </c>
       <c r="F53" s="33">
         <v>26</v>
       </c>
       <c r="G53" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.30232558139534882</v>
       </c>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54" s="10">
-        <f ca="1">1-($G$6-(F54/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.31087299374692567</v>
       </c>
       <c r="F54" s="33">
         <v>27</v>
       </c>
       <c r="G54" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.31034482758620691</v>
       </c>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55" s="10">
-        <f ca="1">1-($G$6-(F55/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.32238680833014521</v>
       </c>
       <c r="F55" s="33">
         <v>28</v>
       </c>
       <c r="G55" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.31818181818181818</v>
       </c>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E56" s="10">
-        <f ca="1">1-($G$6-(F56/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.33390062291336453</v>
       </c>
       <c r="F56" s="33">
         <v>29</v>
       </c>
       <c r="G56" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.3258426966292135</v>
       </c>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E57" s="10">
-        <f ca="1">1-($G$6-(F57/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.34541443749658407</v>
       </c>
       <c r="F57" s="33">
         <v>30</v>
       </c>
       <c r="G57" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E58" s="10">
-        <f ca="1">1-($G$6-(F58/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.3569282520798035</v>
       </c>
       <c r="F58" s="33">
         <v>31</v>
       </c>
       <c r="G58" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.34065934065934067</v>
       </c>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E59" s="10">
-        <f ca="1">1-($G$6-(F59/100))/$G$6</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.36844206666302304</v>
       </c>
       <c r="F59" s="33">
         <v>32</v>
       </c>
       <c r="G59" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.34782608695652173</v>
       </c>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E60" s="10">
-        <f ca="1">1-($G$6-(F60/100))/$G$6</f>
+        <f t="shared" ref="E60:E91" ca="1" si="16">1-($G$6-(F60/100))/$G$6</f>
         <v>0.37995588124624247</v>
       </c>
       <c r="F60" s="33">
         <v>33</v>
       </c>
       <c r="G60" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.35483870967741937</v>
       </c>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E61" s="10">
-        <f ca="1">1-($G$6-(F61/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.39146969582946201</v>
       </c>
       <c r="F61" s="33">
         <v>34</v>
       </c>
       <c r="G61" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.36170212765957449</v>
       </c>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E62" s="10">
-        <f ca="1">1-($G$6-(F62/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.40298351041268143</v>
       </c>
       <c r="F62" s="33">
         <v>35</v>
       </c>
       <c r="G62" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.36842105263157893</v>
       </c>
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E63" s="10">
-        <f ca="1">1-($G$6-(F63/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.41449732499590097</v>
       </c>
       <c r="F63" s="33">
         <v>36</v>
       </c>
       <c r="G63" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.375</v>
       </c>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E64" s="10">
-        <f ca="1">1-($G$6-(F64/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.4260111395791204</v>
       </c>
       <c r="F64" s="33">
         <v>37</v>
       </c>
       <c r="G64" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.38144329896907214</v>
       </c>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E65" s="10">
-        <f ca="1">1-($G$6-(F65/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.43752495416233983</v>
       </c>
       <c r="F65" s="33">
         <v>38</v>
       </c>
       <c r="G65" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.38775510204081631</v>
       </c>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E66" s="10">
-        <f ca="1">1-($G$6-(F66/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.44903876874555937</v>
       </c>
       <c r="F66" s="33">
         <v>39</v>
       </c>
       <c r="G66" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.39393939393939392</v>
       </c>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E67" s="10">
-        <f ca="1">1-($G$6-(F67/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.4605525833287788</v>
       </c>
       <c r="F67" s="33">
         <v>40</v>
       </c>
       <c r="G67" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E68" s="10">
-        <f ca="1">1-($G$6-(F68/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.47206639791199823</v>
       </c>
       <c r="F68" s="33">
         <v>41</v>
       </c>
       <c r="G68" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.40594059405940597</v>
       </c>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E69" s="10">
-        <f ca="1">1-($G$6-(F69/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.48358021249521776</v>
       </c>
       <c r="F69" s="33">
         <v>42</v>
       </c>
       <c r="G69" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.41176470588235292</v>
       </c>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E70" s="10">
-        <f ca="1">1-($G$6-(F70/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.49509402707843719</v>
       </c>
       <c r="F70" s="33">
         <v>43</v>
       </c>
       <c r="G70" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.41747572815533979</v>
       </c>
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E71" s="10">
-        <f ca="1">1-($G$6-(F71/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.50660784166165662</v>
       </c>
       <c r="F71" s="33">
         <v>44</v>
       </c>
       <c r="G71" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.42307692307692307</v>
       </c>
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E72" s="10">
-        <f ca="1">1-($G$6-(F72/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.51812165624487616</v>
       </c>
       <c r="F72" s="33">
         <v>45</v>
       </c>
       <c r="G72" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E73" s="10">
-        <f ca="1">1-($G$6-(F73/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.5296354708280957</v>
       </c>
       <c r="F73" s="33">
         <v>46</v>
       </c>
       <c r="G73" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.43396226415094341</v>
       </c>
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E74" s="10">
-        <f ca="1">1-($G$6-(F74/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.54114928541131513</v>
       </c>
       <c r="F74" s="33">
         <v>47</v>
       </c>
       <c r="G74" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.43925233644859812</v>
       </c>
     </row>
     <row r="75" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E75" s="10">
-        <f ca="1">1-($G$6-(F75/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.55266309999453456</v>
       </c>
       <c r="F75" s="33">
         <v>48</v>
       </c>
       <c r="G75" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E76" s="10">
-        <f ca="1">1-($G$6-(F76/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.56417691457775399</v>
       </c>
       <c r="F76" s="33">
         <v>49</v>
       </c>
       <c r="G76" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.44954128440366975</v>
       </c>
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E77" s="10">
-        <f ca="1">1-($G$6-(F77/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.57569072916097352</v>
       </c>
       <c r="F77" s="33">
         <v>50</v>
       </c>
       <c r="G77" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E78" s="10">
-        <f ca="1">1-($G$6-(F78/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.58720454374419306</v>
       </c>
       <c r="F78" s="33">
         <v>51</v>
       </c>
       <c r="G78" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.45945945945945948</v>
       </c>
     </row>
     <row r="79" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E79" s="10">
-        <f ca="1">1-($G$6-(F79/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.59871835832741249</v>
       </c>
       <c r="F79" s="33">
         <v>52</v>
       </c>
       <c r="G79" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.4642857142857143</v>
       </c>
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E80" s="10">
-        <f ca="1">1-($G$6-(F80/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.61023217291063192</v>
       </c>
       <c r="F80" s="33">
         <v>53</v>
       </c>
       <c r="G80" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.46902654867256638</v>
       </c>
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E81" s="10">
-        <f ca="1">1-($G$6-(F81/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.62174598749385146</v>
       </c>
       <c r="F81" s="33">
         <v>54</v>
       </c>
       <c r="G81" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.47368421052631576</v>
       </c>
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E82" s="10">
-        <f ca="1">1-($G$6-(F82/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.633259802077071</v>
       </c>
       <c r="F82" s="33">
         <v>55</v>
       </c>
       <c r="G82" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.47826086956521741</v>
       </c>
     </row>
     <row r="83" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E83" s="10">
-        <f ca="1">1-($G$6-(F83/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.64477361666029043</v>
       </c>
       <c r="F83" s="33">
         <v>56</v>
       </c>
       <c r="G83" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.48275862068965519</v>
       </c>
     </row>
     <row r="84" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E84" s="10">
-        <f ca="1">1-($G$6-(F84/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.65628743124350974</v>
       </c>
       <c r="F84" s="33">
         <v>57</v>
       </c>
       <c r="G84" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.48717948717948717</v>
       </c>
     </row>
     <row r="85" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E85" s="10">
-        <f ca="1">1-($G$6-(F85/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.66780124582672928</v>
       </c>
       <c r="F85" s="33">
         <v>58</v>
       </c>
       <c r="G85" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.49152542372881358</v>
       </c>
     </row>
     <row r="86" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E86" s="10">
-        <f ca="1">1-($G$6-(F86/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.67931506040994871</v>
       </c>
       <c r="F86" s="33">
         <v>59</v>
       </c>
       <c r="G86" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.49579831932773111</v>
       </c>
     </row>
     <row r="87" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E87" s="10">
-        <f ca="1">1-($G$6-(F87/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.69082887499316814</v>
       </c>
       <c r="F87" s="33">
         <v>60</v>
       </c>
       <c r="G87" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="88" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E88" s="10">
-        <f ca="1">1-($G$6-(F88/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.70234268957638768</v>
       </c>
       <c r="F88" s="33">
         <v>61</v>
       </c>
       <c r="G88" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.50413223140495866</v>
       </c>
     </row>
     <row r="89" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E89" s="10">
-        <f ca="1">1-($G$6-(F89/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.71385650415960722</v>
       </c>
       <c r="F89" s="33">
         <v>62</v>
       </c>
       <c r="G89" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.50819672131147542</v>
       </c>
     </row>
     <row r="90" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E90" s="10">
-        <f ca="1">1-($G$6-(F90/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.72537031874282665</v>
       </c>
       <c r="F90" s="33">
         <v>63</v>
       </c>
       <c r="G90" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.51219512195121952</v>
       </c>
     </row>
     <row r="91" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E91" s="10">
-        <f ca="1">1-($G$6-(F91/100))/$G$6</f>
+        <f t="shared" ca="1" si="16"/>
         <v>0.73688413332604608</v>
       </c>
       <c r="F91" s="33">
         <v>64</v>
       </c>
       <c r="G91" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.5161290322580645</v>
       </c>
     </row>
     <row r="92" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E92" s="10">
-        <f ca="1">1-($G$6-(F92/100))/$G$6</f>
+        <f t="shared" ref="E92:E123" ca="1" si="17">1-($G$6-(F92/100))/$G$6</f>
         <v>0.74839794790926562</v>
       </c>
       <c r="F92" s="33">
         <v>65</v>
       </c>
       <c r="G92" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.52</v>
       </c>
     </row>
     <row r="93" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E93" s="10">
-        <f ca="1">1-($G$6-(F93/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.75991176249248515</v>
       </c>
       <c r="F93" s="33">
         <v>66</v>
       </c>
       <c r="G93" s="10">
-        <f t="shared" ref="G93:G156" si="14">F93/(F93+60)</f>
+        <f t="shared" ref="G93:G156" si="18">F93/(F93+60)</f>
         <v>0.52380952380952384</v>
       </c>
     </row>
     <row r="94" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E94" s="10">
-        <f ca="1">1-($G$6-(F94/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.77142557707570458</v>
       </c>
       <c r="F94" s="33">
         <v>67</v>
       </c>
       <c r="G94" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.52755905511811019</v>
       </c>
     </row>
     <row r="95" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E95" s="10">
-        <f ca="1">1-($G$6-(F95/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.78293939165892401</v>
       </c>
       <c r="F95" s="33">
         <v>68</v>
       </c>
       <c r="G95" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.53125</v>
       </c>
     </row>
     <row r="96" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E96" s="10">
-        <f ca="1">1-($G$6-(F96/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.79445320624214344</v>
       </c>
       <c r="F96" s="33">
         <v>69</v>
       </c>
       <c r="G96" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.53488372093023251</v>
       </c>
     </row>
     <row r="97" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E97" s="10">
-        <f ca="1">1-($G$6-(F97/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.80596702082536287</v>
       </c>
       <c r="F97" s="33">
         <v>70</v>
       </c>
       <c r="G97" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.53846153846153844</v>
       </c>
     </row>
     <row r="98" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E98" s="10">
-        <f ca="1">1-($G$6-(F98/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.8174808354085823</v>
       </c>
       <c r="F98" s="33">
         <v>71</v>
       </c>
       <c r="G98" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.5419847328244275</v>
       </c>
     </row>
     <row r="99" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E99" s="10">
-        <f ca="1">1-($G$6-(F99/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.82899464999180184</v>
       </c>
       <c r="F99" s="33">
         <v>72</v>
       </c>
       <c r="G99" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="100" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E100" s="10">
-        <f ca="1">1-($G$6-(F100/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.84050846457502137</v>
       </c>
       <c r="F100" s="33">
         <v>73</v>
       </c>
       <c r="G100" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.54887218045112784</v>
       </c>
     </row>
     <row r="101" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E101" s="10">
-        <f ca="1">1-($G$6-(F101/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.8520222791582408</v>
       </c>
       <c r="F101" s="33">
         <v>74</v>
       </c>
       <c r="G101" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.55223880597014929</v>
       </c>
     </row>
     <row r="102" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E102" s="10">
-        <f ca="1">1-($G$6-(F102/100))/$G$6</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0.86353609374146023</v>
       </c>
       <c r="F102" s="33">
         <v>75</v>
       </c>
       <c r="G102" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="103" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E103" s="10">
-        <f t="shared" ref="E103:E166" ca="1" si="15">1-($G$6-(F103/100))/$G$6</f>
+        <f t="shared" ref="E103:E166" ca="1" si="19">1-($G$6-(F103/100))/$G$6</f>
         <v>0.87504990832467977</v>
       </c>
       <c r="F103" s="33">
         <v>76</v>
       </c>
       <c r="G103" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.55882352941176472</v>
       </c>
     </row>
     <row r="104" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E104" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.8865637229078992</v>
       </c>
       <c r="F104" s="33">
         <v>77</v>
       </c>
       <c r="G104" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.56204379562043794</v>
       </c>
     </row>
     <row r="105" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E105" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.89807753749111874</v>
       </c>
       <c r="F105" s="33">
         <v>78</v>
       </c>
       <c r="G105" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.56521739130434778</v>
       </c>
     </row>
     <row r="106" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E106" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.90959135207433817</v>
       </c>
       <c r="F106" s="33">
         <v>79</v>
       </c>
       <c r="G106" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.56834532374100721</v>
       </c>
     </row>
     <row r="107" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E107" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.92110516665755771</v>
       </c>
       <c r="F107" s="33">
         <v>80</v>
       </c>
       <c r="G107" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="108" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E108" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.93261898124077713</v>
       </c>
       <c r="F108" s="33">
         <v>81</v>
       </c>
       <c r="G108" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.57446808510638303</v>
       </c>
     </row>
     <row r="109" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E109" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.94413279582399656</v>
       </c>
       <c r="F109" s="33">
         <v>82</v>
       </c>
       <c r="G109" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.57746478873239437</v>
       </c>
     </row>
     <row r="110" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E110" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.95564661040721599</v>
       </c>
       <c r="F110" s="33">
         <v>83</v>
       </c>
       <c r="G110" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.58041958041958042</v>
       </c>
     </row>
     <row r="111" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E111" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.96716042499043553</v>
       </c>
       <c r="F111" s="33">
         <v>84</v>
       </c>
       <c r="G111" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="112" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E112" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.97867423957365496</v>
       </c>
       <c r="F112" s="33">
         <v>85</v>
       </c>
       <c r="G112" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.58620689655172409</v>
       </c>
     </row>
     <row r="113" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E113" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0.9901880541568745</v>
       </c>
       <c r="F113" s="33">
         <v>86</v>
       </c>
       <c r="G113" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.58904109589041098</v>
       </c>
     </row>
     <row r="114" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E114" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.0017018687400938</v>
       </c>
       <c r="F114" s="33">
         <v>87</v>
       </c>
       <c r="G114" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.59183673469387754</v>
       </c>
     </row>
     <row r="115" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E115" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.0132156833233135</v>
       </c>
       <c r="F115" s="33">
         <v>88</v>
       </c>
       <c r="G115" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.59459459459459463</v>
       </c>
     </row>
     <row r="116" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E116" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.0247294979065329</v>
       </c>
       <c r="F116" s="33">
         <v>89</v>
       </c>
       <c r="G116" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.59731543624161076</v>
       </c>
     </row>
     <row r="117" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E117" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.0362433124897523</v>
       </c>
       <c r="F117" s="33">
         <v>90</v>
       </c>
       <c r="G117" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
     </row>
     <row r="118" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E118" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.0477571270729718</v>
       </c>
       <c r="F118" s="33">
         <v>91</v>
       </c>
       <c r="G118" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.60264900662251653</v>
       </c>
     </row>
     <row r="119" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E119" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.0592709416561914</v>
       </c>
       <c r="F119" s="33">
         <v>92</v>
       </c>
       <c r="G119" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.60526315789473684</v>
       </c>
     </row>
     <row r="120" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E120" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.0707847562394108</v>
       </c>
       <c r="F120" s="33">
         <v>93</v>
       </c>
       <c r="G120" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.60784313725490191</v>
       </c>
     </row>
     <row r="121" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E121" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.0822985708226303</v>
       </c>
       <c r="F121" s="33">
         <v>94</v>
       </c>
       <c r="G121" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.61038961038961037</v>
       </c>
     </row>
     <row r="122" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E122" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.0938123854058497</v>
       </c>
       <c r="F122" s="33">
         <v>95</v>
       </c>
       <c r="G122" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.61290322580645162</v>
       </c>
     </row>
     <row r="123" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E123" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.1053261999890691</v>
       </c>
       <c r="F123" s="33">
         <v>96</v>
       </c>
       <c r="G123" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.61538461538461542</v>
       </c>
     </row>
     <row r="124" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E124" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.1168400145722885</v>
       </c>
       <c r="F124" s="33">
         <v>97</v>
       </c>
       <c r="G124" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.61783439490445857</v>
       </c>
     </row>
     <row r="125" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E125" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.128353829155508</v>
       </c>
       <c r="F125" s="33">
         <v>98</v>
       </c>
       <c r="G125" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.620253164556962</v>
       </c>
     </row>
     <row r="126" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E126" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.1398676437387276</v>
       </c>
       <c r="F126" s="33">
         <v>99</v>
       </c>
       <c r="G126" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.62264150943396224</v>
       </c>
     </row>
     <row r="127" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E127" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.151381458321947</v>
       </c>
       <c r="F127" s="33">
         <v>100</v>
       </c>
       <c r="G127" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.625</v>
       </c>
     </row>
     <row r="128" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E128" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.1628952729051665</v>
       </c>
       <c r="F128" s="33">
         <v>101</v>
       </c>
       <c r="G128" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.62732919254658381</v>
       </c>
     </row>
     <row r="129" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E129" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.1744090874883861</v>
       </c>
       <c r="F129" s="33">
         <v>102</v>
       </c>
       <c r="G129" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.62962962962962965</v>
       </c>
     </row>
     <row r="130" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E130" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.1859229020716056</v>
       </c>
       <c r="F130" s="33">
         <v>103</v>
       </c>
       <c r="G130" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.63190184049079756</v>
       </c>
     </row>
     <row r="131" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E131" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.197436716654825</v>
       </c>
       <c r="F131" s="33">
         <v>104</v>
       </c>
       <c r="G131" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.63414634146341464</v>
       </c>
     </row>
     <row r="132" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E132" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.2089505312380444</v>
       </c>
       <c r="F132" s="33">
         <v>105</v>
       </c>
       <c r="G132" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.63636363636363635</v>
       </c>
     </row>
     <row r="133" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E133" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.2204643458212638</v>
       </c>
       <c r="F133" s="33">
         <v>106</v>
       </c>
       <c r="G133" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.63855421686746983</v>
       </c>
     </row>
     <row r="134" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E134" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.2319781604044835</v>
       </c>
       <c r="F134" s="33">
         <v>107</v>
       </c>
       <c r="G134" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.64071856287425155</v>
       </c>
     </row>
     <row r="135" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E135" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.2434919749877029</v>
       </c>
       <c r="F135" s="33">
         <v>108</v>
       </c>
       <c r="G135" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="136" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E136" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.2550057895709223</v>
       </c>
       <c r="F136" s="33">
         <v>109</v>
       </c>
       <c r="G136" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.6449704142011834</v>
       </c>
     </row>
     <row r="137" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E137" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.2665196041541418</v>
       </c>
       <c r="F137" s="33">
         <v>110</v>
       </c>
       <c r="G137" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="138" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E138" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.2780334187373614</v>
       </c>
       <c r="F138" s="33">
         <v>111</v>
       </c>
       <c r="G138" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.64912280701754388</v>
       </c>
     </row>
     <row r="139" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E139" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.2895472333205809</v>
       </c>
       <c r="F139" s="33">
         <v>112</v>
       </c>
       <c r="G139" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.65116279069767447</v>
       </c>
     </row>
     <row r="140" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E140" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.3010610479038001</v>
       </c>
       <c r="F140" s="33">
         <v>113</v>
       </c>
       <c r="G140" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.65317919075144504</v>
       </c>
     </row>
     <row r="141" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E141" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.3125748624870195</v>
       </c>
       <c r="F141" s="33">
         <v>114</v>
       </c>
       <c r="G141" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.65517241379310343</v>
       </c>
     </row>
     <row r="142" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E142" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.3240886770702389</v>
       </c>
       <c r="F142" s="33">
         <v>115</v>
       </c>
       <c r="G142" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.65714285714285714</v>
       </c>
     </row>
     <row r="143" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E143" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.3356024916534586</v>
       </c>
       <c r="F143" s="33">
         <v>116</v>
       </c>
       <c r="G143" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.65909090909090906</v>
       </c>
     </row>
     <row r="144" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E144" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.347116306236678</v>
       </c>
       <c r="F144" s="33">
         <v>117</v>
       </c>
       <c r="G144" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.66101694915254239</v>
       </c>
     </row>
     <row r="145" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E145" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.3586301208198974</v>
       </c>
       <c r="F145" s="33">
         <v>118</v>
       </c>
       <c r="G145" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.6629213483146067</v>
       </c>
     </row>
     <row r="146" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E146" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.3701439354031169</v>
       </c>
       <c r="F146" s="33">
         <v>119</v>
       </c>
       <c r="G146" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.66480446927374304</v>
       </c>
     </row>
     <row r="147" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E147" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.3816577499863363</v>
       </c>
       <c r="F147" s="33">
         <v>120</v>
       </c>
       <c r="G147" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="148" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E148" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.3931715645695559</v>
       </c>
       <c r="F148" s="33">
         <v>121</v>
       </c>
       <c r="G148" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.66850828729281764</v>
       </c>
     </row>
     <row r="149" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E149" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.4046853791527754</v>
       </c>
       <c r="F149" s="33">
         <v>122</v>
       </c>
       <c r="G149" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.67032967032967028</v>
       </c>
     </row>
     <row r="150" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E150" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.4161991937359948</v>
       </c>
       <c r="F150" s="33">
         <v>123</v>
       </c>
       <c r="G150" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.67213114754098358</v>
       </c>
     </row>
     <row r="151" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E151" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.4277130083192144</v>
       </c>
       <c r="F151" s="33">
         <v>124</v>
       </c>
       <c r="G151" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.67391304347826086</v>
       </c>
     </row>
     <row r="152" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E152" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.4392268229024339</v>
       </c>
       <c r="F152" s="33">
         <v>125</v>
       </c>
       <c r="G152" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.67567567567567566</v>
       </c>
     </row>
     <row r="153" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E153" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.4507406374856533</v>
       </c>
       <c r="F153" s="33">
         <v>126</v>
       </c>
       <c r="G153" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.67741935483870963</v>
       </c>
     </row>
     <row r="154" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E154" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.4622544520688727</v>
       </c>
       <c r="F154" s="33">
         <v>127</v>
       </c>
       <c r="G154" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.67914438502673802</v>
       </c>
     </row>
     <row r="155" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E155" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.4737682666520922</v>
       </c>
       <c r="F155" s="33">
         <v>128</v>
       </c>
       <c r="G155" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.68085106382978722</v>
       </c>
     </row>
     <row r="156" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E156" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.4852820812353118</v>
       </c>
       <c r="F156" s="33">
         <v>129</v>
       </c>
       <c r="G156" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.68253968253968256</v>
       </c>
     </row>
     <row r="157" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E157" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.4967958958185312</v>
       </c>
       <c r="F157" s="33">
         <v>130</v>
       </c>
       <c r="G157" s="10">
-        <f t="shared" ref="G157:G220" si="16">F157/(F157+60)</f>
+        <f t="shared" ref="G157:G220" si="20">F157/(F157+60)</f>
         <v>0.68421052631578949</v>
       </c>
     </row>
     <row r="158" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E158" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.5083097104017507</v>
       </c>
       <c r="F158" s="33">
         <v>131</v>
       </c>
       <c r="G158" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.68586387434554974</v>
       </c>
     </row>
     <row r="159" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E159" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.5198235249849703</v>
       </c>
       <c r="F159" s="33">
         <v>132</v>
       </c>
       <c r="G159" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.6875</v>
       </c>
     </row>
     <row r="160" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E160" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.5313373395681897</v>
       </c>
       <c r="F160" s="33">
         <v>133</v>
       </c>
       <c r="G160" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.68911917098445596</v>
       </c>
     </row>
     <row r="161" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E161" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.5428511541514092</v>
       </c>
       <c r="F161" s="33">
         <v>134</v>
       </c>
       <c r="G161" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.69072164948453607</v>
       </c>
     </row>
     <row r="162" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E162" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.5543649687346286</v>
       </c>
       <c r="F162" s="33">
         <v>135</v>
       </c>
       <c r="G162" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.69230769230769229</v>
       </c>
     </row>
     <row r="163" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E163" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.565878783317848</v>
       </c>
       <c r="F163" s="33">
         <v>136</v>
       </c>
       <c r="G163" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.69387755102040816</v>
       </c>
     </row>
     <row r="164" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E164" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.5773925979010675</v>
       </c>
       <c r="F164" s="33">
         <v>137</v>
       </c>
       <c r="G164" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.69543147208121825</v>
       </c>
     </row>
     <row r="165" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E165" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.5889064124842869</v>
       </c>
       <c r="F165" s="33">
         <v>138</v>
       </c>
       <c r="G165" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.69696969696969702</v>
       </c>
     </row>
     <row r="166" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E166" s="10">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="19"/>
         <v>1.6004202270675063</v>
       </c>
       <c r="F166" s="33">
         <v>139</v>
       </c>
       <c r="G166" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.69849246231155782</v>
       </c>
     </row>
     <row r="167" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E167" s="10">
-        <f t="shared" ref="E167:E230" ca="1" si="17">1-($G$6-(F167/100))/$G$6</f>
+        <f t="shared" ref="E167:E230" ca="1" si="21">1-($G$6-(F167/100))/$G$6</f>
         <v>1.6119340416507257</v>
       </c>
       <c r="F167" s="33">
         <v>140</v>
       </c>
       <c r="G167" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.7</v>
       </c>
     </row>
     <row r="168" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E168" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.6234478562339452</v>
       </c>
       <c r="F168" s="33">
         <v>141</v>
       </c>
       <c r="G168" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.70149253731343286</v>
       </c>
     </row>
     <row r="169" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E169" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.6349616708171646</v>
       </c>
       <c r="F169" s="33">
         <v>142</v>
       </c>
       <c r="G169" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.70297029702970293</v>
       </c>
     </row>
     <row r="170" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E170" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.6464754854003842</v>
       </c>
       <c r="F170" s="33">
         <v>143</v>
       </c>
       <c r="G170" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.70443349753694584</v>
       </c>
     </row>
     <row r="171" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E171" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.6579892999836037</v>
       </c>
       <c r="F171" s="33">
         <v>144</v>
       </c>
       <c r="G171" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.70588235294117652</v>
       </c>
     </row>
     <row r="172" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E172" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.6695031145668233</v>
       </c>
       <c r="F172" s="33">
         <v>145</v>
       </c>
       <c r="G172" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.70731707317073167</v>
       </c>
     </row>
     <row r="173" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E173" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.6810169291500427</v>
       </c>
       <c r="F173" s="33">
         <v>146</v>
       </c>
       <c r="G173" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.70873786407766992</v>
       </c>
     </row>
     <row r="174" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E174" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.6925307437332622</v>
       </c>
       <c r="F174" s="33">
         <v>147</v>
       </c>
       <c r="G174" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.71014492753623193</v>
       </c>
     </row>
     <row r="175" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E175" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.7040445583164816</v>
       </c>
       <c r="F175" s="33">
         <v>148</v>
       </c>
       <c r="G175" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.71153846153846156</v>
       </c>
     </row>
     <row r="176" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E176" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.715558372899701</v>
       </c>
       <c r="F176" s="33">
         <v>149</v>
       </c>
       <c r="G176" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.71291866028708128</v>
       </c>
     </row>
     <row r="177" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E177" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.7270721874829205</v>
       </c>
       <c r="F177" s="33">
         <v>150</v>
       </c>
       <c r="G177" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="178" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E178" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.7385860020661399</v>
       </c>
       <c r="F178" s="33">
         <v>151</v>
       </c>
       <c r="G178" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.71563981042654023</v>
       </c>
     </row>
     <row r="179" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E179" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.7500998166493595</v>
       </c>
       <c r="F179" s="33">
         <v>152</v>
       </c>
       <c r="G179" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.71698113207547165</v>
       </c>
     </row>
     <row r="180" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E180" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.761613631232579</v>
       </c>
       <c r="F180" s="33">
         <v>153</v>
       </c>
       <c r="G180" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.71830985915492962</v>
       </c>
     </row>
     <row r="181" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E181" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.7731274458157986</v>
       </c>
       <c r="F181" s="33">
         <v>154</v>
       </c>
       <c r="G181" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.71962616822429903</v>
       </c>
     </row>
     <row r="182" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E182" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.784641260399018</v>
       </c>
       <c r="F182" s="33">
         <v>155</v>
       </c>
       <c r="G182" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.72093023255813948</v>
       </c>
     </row>
     <row r="183" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E183" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.7961550749822375</v>
       </c>
       <c r="F183" s="33">
         <v>156</v>
       </c>
       <c r="G183" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="184" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E184" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.8076688895654569</v>
       </c>
       <c r="F184" s="33">
         <v>157</v>
       </c>
       <c r="G184" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.72350230414746541</v>
       </c>
     </row>
     <row r="185" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E185" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.8191827041486763</v>
       </c>
       <c r="F185" s="33">
         <v>158</v>
       </c>
       <c r="G185" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.72477064220183485</v>
       </c>
     </row>
     <row r="186" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E186" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.8306965187318958</v>
       </c>
       <c r="F186" s="33">
         <v>159</v>
       </c>
       <c r="G186" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.72602739726027399</v>
       </c>
     </row>
     <row r="187" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E187" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.8422103333151154</v>
       </c>
       <c r="F187" s="33">
         <v>160</v>
       </c>
       <c r="G187" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="188" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E188" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.8537241478983348</v>
       </c>
       <c r="F188" s="33">
         <v>161</v>
       </c>
       <c r="G188" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.72850678733031671</v>
       </c>
     </row>
     <row r="189" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E189" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.8652379624815545</v>
       </c>
       <c r="F189" s="33">
         <v>162</v>
       </c>
       <c r="G189" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.72972972972972971</v>
       </c>
     </row>
     <row r="190" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E190" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.8767517770647735</v>
       </c>
       <c r="F190" s="33">
         <v>163</v>
       </c>
       <c r="G190" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.73094170403587444</v>
       </c>
     </row>
     <row r="191" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E191" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.8882655916479929</v>
       </c>
       <c r="F191" s="33">
         <v>164</v>
       </c>
       <c r="G191" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.7321428571428571</v>
       </c>
     </row>
     <row r="192" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E192" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.8997794062312126</v>
       </c>
       <c r="F192" s="33">
         <v>165</v>
       </c>
       <c r="G192" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.73333333333333328</v>
       </c>
     </row>
     <row r="193" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E193" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.911293220814432</v>
       </c>
       <c r="F193" s="33">
         <v>166</v>
       </c>
       <c r="G193" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.73451327433628322</v>
       </c>
     </row>
     <row r="194" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E194" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.9228070353976516</v>
       </c>
       <c r="F194" s="33">
         <v>167</v>
       </c>
       <c r="G194" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.73568281938325997</v>
       </c>
     </row>
     <row r="195" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E195" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.9343208499808711</v>
       </c>
       <c r="F195" s="33">
         <v>168</v>
       </c>
       <c r="G195" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.73684210526315785</v>
       </c>
     </row>
     <row r="196" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E196" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.9458346645640905</v>
       </c>
       <c r="F196" s="33">
         <v>169</v>
       </c>
       <c r="G196" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.73799126637554591</v>
       </c>
     </row>
     <row r="197" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E197" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.9573484791473099</v>
       </c>
       <c r="F197" s="33">
         <v>170</v>
       </c>
       <c r="G197" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.73913043478260865</v>
       </c>
     </row>
     <row r="198" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E198" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.9688622937305293</v>
       </c>
       <c r="F198" s="33">
         <v>171</v>
       </c>
       <c r="G198" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.74025974025974028</v>
       </c>
     </row>
     <row r="199" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E199" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.9803761083137488</v>
       </c>
       <c r="F199" s="33">
         <v>172</v>
       </c>
       <c r="G199" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.74137931034482762</v>
       </c>
     </row>
     <row r="200" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E200" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1.9918899228969684</v>
       </c>
       <c r="F200" s="33">
         <v>173</v>
       </c>
       <c r="G200" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.74248927038626611</v>
       </c>
     </row>
     <row r="201" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E201" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.0034037374801876</v>
       </c>
       <c r="F201" s="33">
         <v>174</v>
       </c>
       <c r="G201" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.74358974358974361</v>
       </c>
     </row>
     <row r="202" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E202" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.0149175520634071</v>
       </c>
       <c r="F202" s="33">
         <v>175</v>
       </c>
       <c r="G202" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.74468085106382975</v>
       </c>
     </row>
     <row r="203" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E203" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.0264313666466265</v>
       </c>
       <c r="F203" s="33">
         <v>176</v>
       </c>
       <c r="G203" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.74576271186440679</v>
       </c>
     </row>
     <row r="204" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E204" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.0379451812298464</v>
       </c>
       <c r="F204" s="33">
         <v>177</v>
       </c>
       <c r="G204" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.74683544303797467</v>
       </c>
     </row>
     <row r="205" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E205" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.0494589958130658</v>
       </c>
       <c r="F205" s="33">
         <v>178</v>
       </c>
       <c r="G205" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.74789915966386555</v>
       </c>
     </row>
     <row r="206" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E206" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.0609728103962852</v>
       </c>
       <c r="F206" s="33">
         <v>179</v>
       </c>
       <c r="G206" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.7489539748953975</v>
       </c>
     </row>
     <row r="207" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E207" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.0724866249795046</v>
       </c>
       <c r="F207" s="33">
         <v>180</v>
       </c>
       <c r="G207" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75</v>
       </c>
     </row>
     <row r="208" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E208" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.0840004395627245</v>
       </c>
       <c r="F208" s="33">
         <v>181</v>
       </c>
       <c r="G208" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75103734439834025</v>
       </c>
     </row>
     <row r="209" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E209" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.0955142541459439</v>
       </c>
       <c r="F209" s="33">
         <v>182</v>
       </c>
       <c r="G209" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75206611570247939</v>
       </c>
     </row>
     <row r="210" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E210" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.1070280687291634</v>
       </c>
       <c r="F210" s="33">
         <v>183</v>
       </c>
       <c r="G210" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75308641975308643</v>
       </c>
     </row>
     <row r="211" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E211" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.1185418833123828</v>
       </c>
       <c r="F211" s="33">
         <v>184</v>
       </c>
       <c r="G211" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75409836065573765</v>
       </c>
     </row>
     <row r="212" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E212" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.1300556978956022</v>
       </c>
       <c r="F212" s="33">
         <v>185</v>
       </c>
       <c r="G212" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75510204081632648</v>
       </c>
     </row>
     <row r="213" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E213" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.1415695124788217</v>
       </c>
       <c r="F213" s="33">
         <v>186</v>
       </c>
       <c r="G213" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75609756097560976</v>
       </c>
     </row>
     <row r="214" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E214" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.1530833270620411</v>
       </c>
       <c r="F214" s="33">
         <v>187</v>
       </c>
       <c r="G214" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75708502024291502</v>
       </c>
     </row>
     <row r="215" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E215" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.1645971416452605</v>
       </c>
       <c r="F215" s="33">
         <v>188</v>
       </c>
       <c r="G215" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75806451612903225</v>
       </c>
     </row>
     <row r="216" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E216" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.1761109562284799</v>
       </c>
       <c r="F216" s="33">
         <v>189</v>
       </c>
       <c r="G216" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.75903614457831325</v>
       </c>
     </row>
     <row r="217" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E217" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.1876247708116994</v>
       </c>
       <c r="F217" s="33">
         <v>190</v>
       </c>
       <c r="G217" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.76</v>
       </c>
     </row>
     <row r="218" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E218" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.1991385853949188</v>
       </c>
       <c r="F218" s="33">
         <v>191</v>
       </c>
       <c r="G218" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.76095617529880477</v>
       </c>
     </row>
     <row r="219" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E219" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.2106523999781382</v>
       </c>
       <c r="F219" s="33">
         <v>192</v>
       </c>
       <c r="G219" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.76190476190476186</v>
       </c>
     </row>
     <row r="220" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E220" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.2221662145613577</v>
       </c>
       <c r="F220" s="33">
         <v>193</v>
       </c>
       <c r="G220" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.76284584980237158</v>
       </c>
     </row>
     <row r="221" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E221" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.2336800291445771</v>
       </c>
       <c r="F221" s="33">
         <v>194</v>
       </c>
       <c r="G221" s="10">
-        <f t="shared" ref="G221:G284" si="18">F221/(F221+60)</f>
+        <f t="shared" ref="G221:G274" si="22">F221/(F221+60)</f>
         <v>0.76377952755905509</v>
       </c>
     </row>
     <row r="222" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E222" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.2451938437277965</v>
       </c>
       <c r="F222" s="33">
         <v>195</v>
       </c>
       <c r="G222" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.76470588235294112</v>
       </c>
     </row>
     <row r="223" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E223" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.2567076583110164</v>
       </c>
       <c r="F223" s="33">
         <v>196</v>
       </c>
       <c r="G223" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.765625</v>
       </c>
     </row>
     <row r="224" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E224" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.2682214728942354</v>
       </c>
       <c r="F224" s="33">
         <v>197</v>
       </c>
       <c r="G224" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.7665369649805448</v>
       </c>
     </row>
     <row r="225" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E225" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.2797352874774552</v>
       </c>
       <c r="F225" s="33">
         <v>198</v>
       </c>
       <c r="G225" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="226" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E226" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.2912491020606742</v>
       </c>
       <c r="F226" s="33">
         <v>199</v>
       </c>
       <c r="G226" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.76833976833976836</v>
       </c>
     </row>
     <row r="227" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E227" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.3027629166438945</v>
       </c>
       <c r="F227" s="33">
         <v>200</v>
       </c>
       <c r="G227" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.76923076923076927</v>
       </c>
     </row>
     <row r="228" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E228" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.3142767312271135</v>
       </c>
       <c r="F228" s="33">
         <v>201</v>
       </c>
       <c r="G228" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77011494252873558</v>
       </c>
     </row>
     <row r="229" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E229" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.3257905458103334</v>
       </c>
       <c r="F229" s="33">
         <v>202</v>
       </c>
       <c r="G229" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77099236641221369</v>
       </c>
     </row>
     <row r="230" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E230" s="10">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="21"/>
         <v>2.3373043603935524</v>
       </c>
       <c r="F230" s="33">
         <v>203</v>
       </c>
       <c r="G230" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77186311787072248</v>
       </c>
     </row>
     <row r="231" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E231" s="10">
-        <f t="shared" ref="E231:E273" ca="1" si="19">1-($G$6-(F231/100))/$G$6</f>
+        <f t="shared" ref="E231:E273" ca="1" si="23">1-($G$6-(F231/100))/$G$6</f>
         <v>2.3488181749767723</v>
       </c>
       <c r="F231" s="33">
         <v>204</v>
       </c>
       <c r="G231" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77272727272727271</v>
       </c>
     </row>
     <row r="232" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E232" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.3603319895599917</v>
       </c>
       <c r="F232" s="33">
         <v>205</v>
       </c>
       <c r="G232" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77358490566037741</v>
       </c>
     </row>
     <row r="233" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E233" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.3718458041432111</v>
       </c>
       <c r="F233" s="33">
         <v>206</v>
       </c>
       <c r="G233" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77443609022556392</v>
       </c>
     </row>
     <row r="234" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E234" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.3833596187264305</v>
       </c>
       <c r="F234" s="33">
         <v>207</v>
       </c>
       <c r="G234" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.7752808988764045</v>
       </c>
     </row>
     <row r="235" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E235" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.39487343330965</v>
       </c>
       <c r="F235" s="33">
         <v>208</v>
       </c>
       <c r="G235" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77611940298507465</v>
       </c>
     </row>
     <row r="236" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E236" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.4063872478928694</v>
       </c>
       <c r="F236" s="33">
         <v>209</v>
       </c>
       <c r="G236" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77695167286245348</v>
       </c>
     </row>
     <row r="237" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E237" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.4179010624760888</v>
       </c>
       <c r="F237" s="33">
         <v>210</v>
       </c>
       <c r="G237" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="238" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E238" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.4294148770593083</v>
       </c>
       <c r="F238" s="33">
         <v>211</v>
       </c>
       <c r="G238" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77859778597785978</v>
       </c>
     </row>
     <row r="239" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E239" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.4409286916425277</v>
       </c>
       <c r="F239" s="33">
         <v>212</v>
       </c>
       <c r="G239" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.77941176470588236</v>
       </c>
     </row>
     <row r="240" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E240" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.4524425062257471</v>
       </c>
       <c r="F240" s="33">
         <v>213</v>
       </c>
       <c r="G240" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78021978021978022</v>
       </c>
     </row>
     <row r="241" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E241" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.463956320808967</v>
       </c>
       <c r="F241" s="33">
         <v>214</v>
       </c>
       <c r="G241" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78102189781021902</v>
       </c>
     </row>
     <row r="242" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E242" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.475470135392186</v>
       </c>
       <c r="F242" s="33">
         <v>215</v>
       </c>
       <c r="G242" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78181818181818186</v>
       </c>
     </row>
     <row r="243" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E243" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.4869839499754058</v>
       </c>
       <c r="F243" s="33">
         <v>216</v>
       </c>
       <c r="G243" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78260869565217395</v>
       </c>
     </row>
     <row r="244" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E244" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.4984977645586248</v>
       </c>
       <c r="F244" s="33">
         <v>217</v>
       </c>
       <c r="G244" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78339350180505418</v>
       </c>
     </row>
     <row r="245" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E245" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.5100115791418451</v>
       </c>
       <c r="F245" s="33">
         <v>218</v>
       </c>
       <c r="G245" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78417266187050361</v>
       </c>
     </row>
     <row r="246" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E246" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.5215253937250641</v>
       </c>
       <c r="F246" s="33">
         <v>219</v>
       </c>
       <c r="G246" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78494623655913975</v>
       </c>
     </row>
     <row r="247" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E247" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.533039208308284</v>
       </c>
       <c r="F247" s="33">
         <v>220</v>
       </c>
       <c r="G247" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.7857142857142857</v>
       </c>
     </row>
     <row r="248" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E248" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.544553022891503</v>
       </c>
       <c r="F248" s="33">
         <v>221</v>
       </c>
       <c r="G248" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78647686832740216</v>
       </c>
     </row>
     <row r="249" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E249" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.5560668374747229</v>
       </c>
       <c r="F249" s="33">
         <v>222</v>
       </c>
       <c r="G249" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78723404255319152</v>
       </c>
     </row>
     <row r="250" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E250" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.5675806520579423</v>
       </c>
       <c r="F250" s="33">
         <v>223</v>
       </c>
       <c r="G250" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78798586572438167</v>
       </c>
     </row>
     <row r="251" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E251" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.5790944666411617</v>
       </c>
       <c r="F251" s="33">
         <v>224</v>
       </c>
       <c r="G251" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78873239436619713</v>
       </c>
     </row>
     <row r="252" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E252" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.5906082812243811</v>
       </c>
       <c r="F252" s="33">
         <v>225</v>
       </c>
       <c r="G252" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.78947368421052633</v>
       </c>
     </row>
     <row r="253" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E253" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.6021220958076001</v>
       </c>
       <c r="F253" s="33">
         <v>226</v>
       </c>
       <c r="G253" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79020979020979021</v>
       </c>
     </row>
     <row r="254" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E254" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.61363591039082</v>
       </c>
       <c r="F254" s="33">
         <v>227</v>
       </c>
       <c r="G254" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.7909407665505227</v>
       </c>
     </row>
     <row r="255" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E255" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.6251497249740394</v>
       </c>
       <c r="F255" s="33">
         <v>228</v>
       </c>
       <c r="G255" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="256" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E256" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.6366635395572589</v>
       </c>
       <c r="F256" s="33">
         <v>229</v>
       </c>
       <c r="G256" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79238754325259519</v>
       </c>
     </row>
     <row r="257" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E257" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.6481773541404783</v>
       </c>
       <c r="F257" s="33">
         <v>230</v>
       </c>
       <c r="G257" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.7931034482758621</v>
       </c>
     </row>
     <row r="258" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E258" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.6596911687236977</v>
       </c>
       <c r="F258" s="33">
         <v>231</v>
       </c>
       <c r="G258" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79381443298969068</v>
       </c>
     </row>
     <row r="259" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E259" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.6712049833069171</v>
       </c>
       <c r="F259" s="33">
         <v>232</v>
       </c>
       <c r="G259" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79452054794520544</v>
       </c>
     </row>
     <row r="260" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E260" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.6827187978901366</v>
       </c>
       <c r="F260" s="33">
         <v>233</v>
       </c>
       <c r="G260" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79522184300341292</v>
       </c>
     </row>
     <row r="261" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E261" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.694232612473356</v>
       </c>
       <c r="F261" s="33">
         <v>234</v>
       </c>
       <c r="G261" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79591836734693877</v>
       </c>
     </row>
     <row r="262" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E262" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.7057464270565759</v>
       </c>
       <c r="F262" s="33">
         <v>235</v>
       </c>
       <c r="G262" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79661016949152541</v>
       </c>
     </row>
     <row r="263" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E263" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.7172602416397948</v>
       </c>
       <c r="F263" s="33">
         <v>236</v>
       </c>
       <c r="G263" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79729729729729726</v>
       </c>
     </row>
     <row r="264" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E264" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.7287740562230147</v>
       </c>
       <c r="F264" s="33">
         <v>237</v>
       </c>
       <c r="G264" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79797979797979801</v>
       </c>
     </row>
     <row r="265" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E265" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.7402878708062337</v>
       </c>
       <c r="F265" s="33">
         <v>238</v>
       </c>
       <c r="G265" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79865771812080533</v>
       </c>
     </row>
     <row r="266" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E266" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.751801685389454</v>
       </c>
       <c r="F266" s="33">
         <v>239</v>
       </c>
       <c r="G266" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.79933110367892979</v>
       </c>
     </row>
     <row r="267" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E267" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.763315499972673</v>
       </c>
       <c r="F267" s="33">
         <v>240</v>
       </c>
       <c r="G267" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.8</v>
       </c>
     </row>
     <row r="268" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E268" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.7748293145558929</v>
       </c>
       <c r="F268" s="33">
         <v>241</v>
       </c>
       <c r="G268" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.80066445182724255</v>
       </c>
     </row>
     <row r="269" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E269" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.7863431291391119</v>
       </c>
       <c r="F269" s="33">
         <v>242</v>
       </c>
       <c r="G269" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.80132450331125826</v>
       </c>
     </row>
     <row r="270" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E270" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.7978569437223317</v>
       </c>
       <c r="F270" s="33">
         <v>243</v>
       </c>
       <c r="G270" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.80198019801980203</v>
       </c>
     </row>
     <row r="271" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E271" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.8093707583055512</v>
       </c>
       <c r="F271" s="33">
         <v>244</v>
       </c>
       <c r="G271" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.80263157894736847</v>
       </c>
     </row>
     <row r="272" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E272" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.8208845728887706</v>
       </c>
       <c r="F272" s="33">
         <v>245</v>
       </c>
       <c r="G272" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.80327868852459017</v>
       </c>
     </row>
     <row r="273" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E273" s="10">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="23"/>
         <v>2.83239838747199</v>
       </c>
       <c r="F273" s="33">
         <v>246</v>
       </c>
       <c r="G273" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.80392156862745101</v>
       </c>
     </row>
@@ -37765,7 +37765,7 @@
         <v>247</v>
       </c>
       <c r="G274" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.80456026058631924</v>
       </c>
     </row>
@@ -38030,8 +38030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q179"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="P157" sqref="P157"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38133,7 +38133,7 @@
         <v>146</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="36"/>
+      <c r="P4" s="37"/>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -38162,7 +38162,7 @@
         <v>147</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="37"/>
+      <c r="P5" s="38"/>
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -38211,7 +38211,7 @@
       <c r="O6" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="P6" s="37"/>
+      <c r="P6" s="38"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -38232,7 +38232,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="37"/>
+      <c r="P7" s="38"/>
       <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
put artificial floor on AP so that AI will still use lasers, they are now OP, but only in very rare circumstances
</commit_message>
<xml_diff>
--- a/Stellaris Rebalance.xlsx
+++ b/Stellaris Rebalance.xlsx
@@ -35396,7 +35396,7 @@
     </row>
     <row r="92" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E92" s="10">
-        <f t="shared" ref="E92:E123" ca="1" si="17">1-($G$6-(F92/100))/$G$6</f>
+        <f t="shared" ref="E92:E102" ca="1" si="17">1-($G$6-(F92/100))/$G$6</f>
         <v>0.74839794790926562</v>
       </c>
       <c r="F92" s="33">
@@ -38030,13 +38030,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="I181" sqref="I181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -38263,8 +38263,8 @@
         <v>0</v>
       </c>
       <c r="H8" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A8,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H8),2)</f>
-        <v>-5.61</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A8,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H8),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A8,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H8),2))</f>
+        <v>-4</v>
       </c>
       <c r="I8" s="5">
         <v>2</v>
@@ -38319,8 +38319,8 @@
         <v>0</v>
       </c>
       <c r="H9" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A9,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H9),2)</f>
-        <v>-8.24</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A9,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H9),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A9,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H9),2))</f>
+        <v>-4</v>
       </c>
       <c r="I9" s="5">
         <v>2</v>
@@ -38375,8 +38375,8 @@
         <v>0</v>
       </c>
       <c r="H10" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A10,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H10),2)</f>
-        <v>-10.63</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A10,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H10),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A10,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H10),2))</f>
+        <v>-4</v>
       </c>
       <c r="I10" s="5">
         <v>2</v>
@@ -38431,7 +38431,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A11,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H11),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A11,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H11),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A11,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H11),2))</f>
         <v>-1.36</v>
       </c>
       <c r="I11" s="5">
@@ -38487,7 +38487,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A12,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H12),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A12,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H12),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A12,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H12),2))</f>
         <v>-1.84</v>
       </c>
       <c r="I12" s="5">
@@ -38543,7 +38543,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A13,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H13),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A13,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H13),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A13,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H13),2))</f>
         <v>-2.29</v>
       </c>
       <c r="I13" s="5">
@@ -38599,7 +38599,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A14,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H14),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A14,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H14),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A14,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H14),2))</f>
         <v>-0.86</v>
       </c>
       <c r="I14" s="5">
@@ -38655,7 +38655,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A15,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H15),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A15,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H15),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A15,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H15),2))</f>
         <v>-1.1000000000000001</v>
       </c>
       <c r="I15" s="5">
@@ -38711,7 +38711,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A16,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H16),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A16,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H16),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A16,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H16),2))</f>
         <v>-1.32</v>
       </c>
       <c r="I16" s="5">
@@ -38767,7 +38767,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A17,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H17),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A17,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H17),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A17,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H17),2))</f>
         <v>-1.06</v>
       </c>
       <c r="I17" s="5">
@@ -38823,7 +38823,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A18,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H18),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A18,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H18),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A18,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H18),2))</f>
         <v>-1.24</v>
       </c>
       <c r="I18" s="5">
@@ -38879,7 +38879,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A19,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H19),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A19,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H19),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A19,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H19),2))</f>
         <v>-1.41</v>
       </c>
       <c r="I19" s="5">
@@ -38935,7 +38935,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A20,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H20),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A20,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H20),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A20,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H20),2))</f>
         <v>-1.03</v>
       </c>
       <c r="I20" s="5">
@@ -38991,7 +38991,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A21,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H21),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A21,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H21),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A21,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H21),2))</f>
         <v>-1.1599999999999999</v>
       </c>
       <c r="I21" s="5">
@@ -39047,7 +39047,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A22,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H22),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A22,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H22),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A22,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H22),2))</f>
         <v>-1.27</v>
       </c>
       <c r="I22" s="5">
@@ -39124,7 +39124,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A24,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H24),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A24,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H24),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A24,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H24),2))</f>
         <v>0.5</v>
       </c>
       <c r="I24" s="5">
@@ -39180,7 +39180,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A25,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H25),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A25,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H25),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A25,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H25),2))</f>
         <v>0.5</v>
       </c>
       <c r="I25" s="5">
@@ -39236,7 +39236,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A26,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H26),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A26,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H26),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A26,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H26),2))</f>
         <v>0.5</v>
       </c>
       <c r="I26" s="5">
@@ -39313,7 +39313,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A28,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H28),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A28,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H28),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A28,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H28),2))</f>
         <v>3.25</v>
       </c>
       <c r="I28" s="5">
@@ -39369,7 +39369,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A29,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H29),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A29,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H29),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A29,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H29),2))</f>
         <v>3.13</v>
       </c>
       <c r="I29" s="5">
@@ -39446,7 +39446,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A31,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H31),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A31,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H31),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A31,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H31),2))</f>
         <v>1.82</v>
       </c>
       <c r="I31" s="5">
@@ -39502,7 +39502,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A32,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H32),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A32,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H32),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A32,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H32),2))</f>
         <v>2.4500000000000002</v>
       </c>
       <c r="I32" s="5">
@@ -39558,7 +39558,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A33,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H33),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A33,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H33),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A33,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H33),2))</f>
         <v>3.21</v>
       </c>
       <c r="I33" s="5">
@@ -39614,7 +39614,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A34,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H34),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A34,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H34),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A34,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H34),2))</f>
         <v>1.93</v>
       </c>
       <c r="I34" s="5">
@@ -39670,7 +39670,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A35,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H35),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A35,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H35),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A35,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H35),2))</f>
         <v>2.52</v>
       </c>
       <c r="I35" s="5">
@@ -39726,7 +39726,7 @@
         <v>0</v>
       </c>
       <c r="H36" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A36,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H36),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A36,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H36),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A36,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H36),2))</f>
         <v>3.25</v>
       </c>
       <c r="I36" s="5">
@@ -39782,7 +39782,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A37,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H37),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A37,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H37),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A37,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H37),2))</f>
         <v>1.96</v>
       </c>
       <c r="I37" s="5">
@@ -39838,7 +39838,7 @@
         <v>0</v>
       </c>
       <c r="H38" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A38,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H38),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A38,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H38),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A38,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H38),2))</f>
         <v>2.48</v>
       </c>
       <c r="I38" s="5">
@@ -39894,7 +39894,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A39,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H39),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A39,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H39),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A39,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H39),2))</f>
         <v>3.13</v>
       </c>
       <c r="I39" s="5">
@@ -39971,7 +39971,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A41,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H41),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A41,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H41),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A41,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H41),2))</f>
         <v>-1.41</v>
       </c>
       <c r="I41" s="5">
@@ -40027,7 +40027,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A42,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H42),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A42,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H42),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A42,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H42),2))</f>
         <v>-1.27</v>
       </c>
       <c r="I42" s="5">
@@ -40104,7 +40104,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A44,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H44),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A44,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H44),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A44,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H44),2))</f>
         <v>-1.78</v>
       </c>
       <c r="I44" s="5">
@@ -40160,7 +40160,7 @@
         <v>0</v>
       </c>
       <c r="H45" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A45,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H45),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A45,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H45),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A45,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H45),2))</f>
         <v>-1.81</v>
       </c>
       <c r="I45" s="5">
@@ -40216,7 +40216,7 @@
         <v>0</v>
       </c>
       <c r="H46" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A46,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H46),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A46,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H46),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A46,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H46),2))</f>
         <v>-1.86</v>
       </c>
       <c r="I46" s="5">
@@ -40272,7 +40272,7 @@
         <v>0</v>
       </c>
       <c r="H47" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A47,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H47),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A47,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H47),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A47,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H47),2))</f>
         <v>-1.65</v>
       </c>
       <c r="I47" s="5">
@@ -40328,7 +40328,7 @@
         <v>0</v>
       </c>
       <c r="H48" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A48,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H48),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A48,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H48),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A48,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H48),2))</f>
         <v>-1.69</v>
       </c>
       <c r="I48" s="5">
@@ -40384,7 +40384,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A49,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H49),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A49,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H49),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A49,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H49),2))</f>
         <v>-1.75</v>
       </c>
       <c r="I49" s="5">
@@ -40440,7 +40440,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A50,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H50),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A50,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H50),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A50,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H50),2))</f>
         <v>-1.37</v>
       </c>
       <c r="I50" s="5">
@@ -40496,7 +40496,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A51,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H51),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A51,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H51),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A51,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H51),2))</f>
         <v>-1.42</v>
       </c>
       <c r="I51" s="5">
@@ -40552,7 +40552,7 @@
         <v>0</v>
       </c>
       <c r="H52" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A52,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H52),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A52,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H52),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A52,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H52),2))</f>
         <v>-1.48</v>
       </c>
       <c r="I52" s="5">
@@ -40629,7 +40629,7 @@
         <v>0</v>
       </c>
       <c r="H54" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A54,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H54),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A54,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H54),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A54,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H54),2))</f>
         <v>-1.0900000000000001</v>
       </c>
       <c r="I54" s="5">
@@ -40685,7 +40685,7 @@
         <v>0</v>
       </c>
       <c r="H55" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A55,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H55),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A55,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H55),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A55,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H55),2))</f>
         <v>-1.01</v>
       </c>
       <c r="I55" s="5">
@@ -40762,8 +40762,8 @@
         <v>1</v>
       </c>
       <c r="H57" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A57,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H57),2)</f>
-        <v>-18.32</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A57,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H57),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A57,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H57),2))</f>
+        <v>-4</v>
       </c>
       <c r="I57" s="5">
         <v>2</v>
@@ -40818,8 +40818,8 @@
         <v>1</v>
       </c>
       <c r="H58" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A58,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H58),2)</f>
-        <v>-13.48</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A58,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H58),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A58,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H58),2))</f>
+        <v>-4</v>
       </c>
       <c r="I58" s="5">
         <v>2</v>
@@ -40874,8 +40874,8 @@
         <v>1</v>
       </c>
       <c r="H59" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A59,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H59),2)</f>
-        <v>-6.83</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A59,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H59),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A59,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H59),2))</f>
+        <v>-4</v>
       </c>
       <c r="I59" s="5">
         <v>2</v>
@@ -40930,7 +40930,7 @@
         <v>1</v>
       </c>
       <c r="H60" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A60,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H60),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A60,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H60),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A60,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H60),2))</f>
         <v>-3.4</v>
       </c>
       <c r="I60" s="5">
@@ -40986,7 +40986,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A61,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H61),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A61,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H61),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A61,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H61),2))</f>
         <v>-2.44</v>
       </c>
       <c r="I61" s="5">
@@ -41042,7 +41042,7 @@
         <v>1</v>
       </c>
       <c r="H62" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A62,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H62),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A62,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H62),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A62,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H62),2))</f>
         <v>-1.17</v>
       </c>
       <c r="I62" s="5">
@@ -41098,7 +41098,7 @@
         <v>1</v>
       </c>
       <c r="H63" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A63,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H63),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A63,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H63),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A63,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H63),2))</f>
         <v>-1.7</v>
       </c>
       <c r="I63" s="5">
@@ -41154,7 +41154,7 @@
         <v>1</v>
       </c>
       <c r="H64" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A64,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H64),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A64,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H64),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A64,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H64),2))</f>
         <v>-1.18</v>
       </c>
       <c r="I64" s="5">
@@ -41210,7 +41210,7 @@
         <v>1</v>
       </c>
       <c r="H65" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A65,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H65),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A65,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H65),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A65,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H65),2))</f>
         <v>-0.5</v>
       </c>
       <c r="I65" s="5">
@@ -41266,7 +41266,7 @@
         <v>1</v>
       </c>
       <c r="H66" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A66,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H66),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A66,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H66),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A66,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H66),2))</f>
         <v>-1.56</v>
       </c>
       <c r="I66" s="5">
@@ -41322,7 +41322,7 @@
         <v>1</v>
       </c>
       <c r="H67" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A67,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H67),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A67,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H67),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A67,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H67),2))</f>
         <v>-1.1000000000000001</v>
       </c>
       <c r="I67" s="5">
@@ -41378,7 +41378,7 @@
         <v>1</v>
       </c>
       <c r="H68" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A68,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H68),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A68,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H68),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A68,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H68),2))</f>
         <v>-0.54</v>
       </c>
       <c r="I68" s="5">
@@ -41434,7 +41434,7 @@
         <v>1</v>
       </c>
       <c r="H69" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A69,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H69),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A69,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H69),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A69,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H69),2))</f>
         <v>-1.27</v>
       </c>
       <c r="I69" s="5">
@@ -41490,7 +41490,7 @@
         <v>1</v>
       </c>
       <c r="H70" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A70,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H70),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A70,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H70),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A70,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H70),2))</f>
         <v>-0.92</v>
       </c>
       <c r="I70" s="5">
@@ -41546,7 +41546,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A71,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H71),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A71,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H71),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A71,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H71),2))</f>
         <v>-0.45</v>
       </c>
       <c r="I71" s="5">
@@ -41623,7 +41623,7 @@
         <v>0</v>
       </c>
       <c r="H73" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A73,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H73),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A73,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H73),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A73,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H73),2))</f>
         <v>0</v>
       </c>
       <c r="I73" s="5">
@@ -41679,7 +41679,7 @@
         <v>0</v>
       </c>
       <c r="H74" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A74,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H74),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A74,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H74),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A74,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H74),2))</f>
         <v>0</v>
       </c>
       <c r="I74" s="5">
@@ -41735,7 +41735,7 @@
         <v>0</v>
       </c>
       <c r="H75" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A75,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H75),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A75,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H75),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A75,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H75),2))</f>
         <v>0</v>
       </c>
       <c r="I75" s="5">
@@ -41812,7 +41812,7 @@
         <v>0</v>
       </c>
       <c r="H77" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A77,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H77),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A77,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H77),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A77,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H77),2))</f>
         <v>-1.91</v>
       </c>
       <c r="I77" s="5">
@@ -41868,7 +41868,7 @@
         <v>0</v>
       </c>
       <c r="H78" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A78,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H78),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A78,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H78),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A78,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H78),2))</f>
         <v>-1.57</v>
       </c>
       <c r="I78" s="5">
@@ -41945,7 +41945,7 @@
         <v>1</v>
       </c>
       <c r="H80" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A80,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H80),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A80,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H80),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A80,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H80),2))</f>
         <v>0.4</v>
       </c>
       <c r="I80" s="5">
@@ -42001,7 +42001,7 @@
         <v>1</v>
       </c>
       <c r="H81" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A81,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H81),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A81,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H81),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A81,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H81),2))</f>
         <v>1.7</v>
       </c>
       <c r="I81" s="5">
@@ -42057,7 +42057,7 @@
         <v>1</v>
       </c>
       <c r="H82" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A82,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H82),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A82,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H82),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A82,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H82),2))</f>
         <v>3.7</v>
       </c>
       <c r="I82" s="5">
@@ -42113,7 +42113,7 @@
         <v>1</v>
       </c>
       <c r="H83" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A83,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H83),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A83,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H83),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A83,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H83),2))</f>
         <v>0.18</v>
       </c>
       <c r="I83" s="5">
@@ -42169,7 +42169,7 @@
         <v>1</v>
       </c>
       <c r="H84" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A84,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H84),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A84,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H84),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A84,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H84),2))</f>
         <v>1.18</v>
       </c>
       <c r="I84" s="5">
@@ -42225,7 +42225,7 @@
         <v>1</v>
       </c>
       <c r="H85" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A85,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H85),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A85,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H85),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A85,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H85),2))</f>
         <v>2.64</v>
       </c>
       <c r="I85" s="5">
@@ -42281,7 +42281,7 @@
         <v>1</v>
       </c>
       <c r="H86" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A86,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H86),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A86,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H86),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A86,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H86),2))</f>
         <v>0.1</v>
       </c>
       <c r="I86" s="5">
@@ -42337,7 +42337,7 @@
         <v>1</v>
       </c>
       <c r="H87" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A87,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H87),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A87,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H87),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A87,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H87),2))</f>
         <v>0.84</v>
       </c>
       <c r="I87" s="5">
@@ -42393,7 +42393,7 @@
         <v>1</v>
       </c>
       <c r="H88" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A88,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H88),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A88,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H88),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A88,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H88),2))</f>
         <v>1.87</v>
       </c>
       <c r="I88" s="5">
@@ -42468,7 +42468,7 @@
         <v>0</v>
       </c>
       <c r="H90" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A90,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H90),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A90,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H90),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A90,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H90),2))</f>
         <v>-1.41</v>
       </c>
       <c r="I90" s="5">
@@ -42522,7 +42522,7 @@
         <v>0</v>
       </c>
       <c r="H91" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A91,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H91),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A91,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H91),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A91,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H91),2))</f>
         <v>-1.27</v>
       </c>
       <c r="I91" s="5">
@@ -42599,7 +42599,7 @@
         <v>1</v>
       </c>
       <c r="H93" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A93,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H93),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A93,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H93),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A93,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H93),2))</f>
         <v>-4</v>
       </c>
       <c r="I93" s="5">
@@ -42655,8 +42655,8 @@
         <v>1</v>
       </c>
       <c r="H94" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A94,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H94),2)</f>
-        <v>-6.86</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A94,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H94),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A94,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H94),2))</f>
+        <v>-4</v>
       </c>
       <c r="I94" s="5">
         <v>20</v>
@@ -42711,8 +42711,8 @@
         <v>1</v>
       </c>
       <c r="H95" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A95,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H95),2)</f>
-        <v>-9.4499999999999993</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A95,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H95),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A95,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H95),2))</f>
+        <v>-4</v>
       </c>
       <c r="I95" s="5">
         <v>20</v>
@@ -42767,7 +42767,7 @@
         <v>1</v>
       </c>
       <c r="H96" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A96,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H96),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A96,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H96),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A96,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H96),2))</f>
         <v>-0.75</v>
       </c>
       <c r="I96" s="5">
@@ -42823,7 +42823,7 @@
         <v>1</v>
       </c>
       <c r="H97" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A97,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H97),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A97,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H97),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A97,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H97),2))</f>
         <v>-1.32</v>
       </c>
       <c r="I97" s="5">
@@ -42879,7 +42879,7 @@
         <v>1</v>
       </c>
       <c r="H98" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A98,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H98),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A98,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H98),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A98,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H98),2))</f>
         <v>-1.85</v>
       </c>
       <c r="I98" s="5">
@@ -42935,7 +42935,7 @@
         <v>1</v>
       </c>
       <c r="H99" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A99,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H99),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A99,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H99),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A99,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H99),2))</f>
         <v>-0.39</v>
       </c>
       <c r="I99" s="5">
@@ -42991,7 +42991,7 @@
         <v>1</v>
       </c>
       <c r="H100" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A100,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H100),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A100,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H100),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A100,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H100),2))</f>
         <v>-0.71</v>
       </c>
       <c r="I100" s="5">
@@ -43047,7 +43047,7 @@
         <v>1</v>
       </c>
       <c r="H101" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A101,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H101),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A101,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H101),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A101,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H101),2))</f>
         <v>-1</v>
       </c>
       <c r="I101" s="5">
@@ -43103,7 +43103,7 @@
         <v>1</v>
       </c>
       <c r="H102" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A102,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H102),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A102,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H102),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A102,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H102),2))</f>
         <v>-0.57999999999999996</v>
       </c>
       <c r="I102" s="5">
@@ -43159,7 +43159,7 @@
         <v>1</v>
       </c>
       <c r="H103" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A103,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H103),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A103,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H103),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A103,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H103),2))</f>
         <v>-0.85</v>
       </c>
       <c r="I103" s="5">
@@ -43215,7 +43215,7 @@
         <v>1</v>
       </c>
       <c r="H104" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A104,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H104),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A104,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H104),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A104,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H104),2))</f>
         <v>-1.0900000000000001</v>
       </c>
       <c r="I104" s="5">
@@ -43271,7 +43271,7 @@
         <v>1</v>
       </c>
       <c r="H105" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A105,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H105),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A105,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H105),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A105,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H105),2))</f>
         <v>-0.6</v>
       </c>
       <c r="I105" s="5">
@@ -43327,7 +43327,7 @@
         <v>1</v>
       </c>
       <c r="H106" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A106,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H106),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A106,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H106),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A106,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H106),2))</f>
         <v>-0.81</v>
       </c>
       <c r="I106" s="5">
@@ -43383,7 +43383,7 @@
         <v>1</v>
       </c>
       <c r="H107" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A107,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H107),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A107,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H107),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A107,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H107),2))</f>
         <v>-1.01</v>
       </c>
       <c r="I107" s="5">
@@ -43460,7 +43460,7 @@
         <v>0</v>
       </c>
       <c r="H109" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A109,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H109),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A109,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H109),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A109,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H109),2))</f>
         <v>0</v>
       </c>
       <c r="I109" s="5">
@@ -43516,7 +43516,7 @@
         <v>0</v>
       </c>
       <c r="H110" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A110,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H110),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A110,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H110),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A110,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H110),2))</f>
         <v>0</v>
       </c>
       <c r="I110" s="5">
@@ -43572,7 +43572,7 @@
         <v>0</v>
       </c>
       <c r="H111" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A111,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H111),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A111,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H111),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A111,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H111),2))</f>
         <v>0</v>
       </c>
       <c r="I111" s="5">
@@ -43649,7 +43649,7 @@
         <v>0.76</v>
       </c>
       <c r="H113" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A113,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H113),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A113,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H113),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A113,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H113),2))</f>
         <v>0.21</v>
       </c>
       <c r="I113">
@@ -43702,7 +43702,7 @@
         <v>0.74</v>
       </c>
       <c r="H114" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A114,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H114),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A114,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H114),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A114,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H114),2))</f>
         <v>-0.13</v>
       </c>
       <c r="I114">
@@ -43755,7 +43755,7 @@
         <v>0.72</v>
       </c>
       <c r="H115" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A115,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H115),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A115,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H115),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A115,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H115),2))</f>
         <v>-0.44</v>
       </c>
       <c r="I115">
@@ -43808,7 +43808,7 @@
         <v>0.74</v>
       </c>
       <c r="H116" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A116,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H116),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A116,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H116),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A116,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H116),2))</f>
         <v>-0.04</v>
       </c>
       <c r="I116">
@@ -43861,7 +43861,7 @@
         <v>0.72</v>
       </c>
       <c r="H117" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A117,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H117),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A117,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H117),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A117,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H117),2))</f>
         <v>-0.33</v>
       </c>
       <c r="I117">
@@ -43914,7 +43914,7 @@
         <v>0.7</v>
       </c>
       <c r="H118" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A118,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H118),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A118,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H118),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A118,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H118),2))</f>
         <v>-0.6</v>
       </c>
       <c r="I118">
@@ -43967,7 +43967,7 @@
         <v>0.72</v>
       </c>
       <c r="H119" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A119,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H119),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A119,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H119),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A119,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H119),2))</f>
         <v>-0.16</v>
       </c>
       <c r="I119">
@@ -44020,7 +44020,7 @@
         <v>0.7</v>
       </c>
       <c r="H120" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A120,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H120),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A120,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H120),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A120,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H120),2))</f>
         <v>-0.39</v>
       </c>
       <c r="I120">
@@ -44073,7 +44073,7 @@
         <v>0.68</v>
       </c>
       <c r="H121" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A121,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H121),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A121,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H121),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A121,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H121),2))</f>
         <v>-0.6</v>
       </c>
       <c r="I121">
@@ -44140,7 +44140,7 @@
         <v>1</v>
       </c>
       <c r="H123" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A123,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H123),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A123,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H123),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A123,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H123),2))</f>
         <v>-0.85</v>
       </c>
       <c r="I123">
@@ -44193,7 +44193,7 @@
         <v>1</v>
       </c>
       <c r="H124" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A124,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H124),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A124,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H124),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A124,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H124),2))</f>
         <v>-0.81</v>
       </c>
       <c r="I124">
@@ -44260,8 +44260,8 @@
         <v>0.2</v>
       </c>
       <c r="H126" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A126,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H126),2)</f>
-        <v>-5.61</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A126,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H126),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A126,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H126),2))</f>
+        <v>-4</v>
       </c>
       <c r="I126">
         <v>2</v>
@@ -44313,8 +44313,8 @@
         <v>0.18</v>
       </c>
       <c r="H127" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A127,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H127),2)</f>
-        <v>-8.24</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A127,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H127),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A127,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H127),2))</f>
+        <v>-4</v>
       </c>
       <c r="I127">
         <v>2</v>
@@ -44380,7 +44380,7 @@
         <v>0</v>
       </c>
       <c r="H129" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A129,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H129),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A129,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H129),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A129,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H129),2))</f>
         <v>4.3899999999999997</v>
       </c>
       <c r="I129">
@@ -44433,7 +44433,7 @@
         <v>0</v>
       </c>
       <c r="H130" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A130,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H130),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A130,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H130),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A130,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H130),2))</f>
         <v>8.7899999999999991</v>
       </c>
       <c r="I130">
@@ -44486,7 +44486,7 @@
         <v>0</v>
       </c>
       <c r="H131" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A131,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H131),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A131,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H131),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A131,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H131),2))</f>
         <v>14.16</v>
       </c>
       <c r="I131">
@@ -44539,7 +44539,7 @@
         <v>0</v>
       </c>
       <c r="H132" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A132,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H132),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A132,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H132),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A132,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H132),2))</f>
         <v>4.3899999999999997</v>
       </c>
       <c r="I132">
@@ -44592,7 +44592,7 @@
         <v>0</v>
       </c>
       <c r="H133" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A133,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H133),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A133,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H133),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A133,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H133),2))</f>
         <v>8.7899999999999991</v>
       </c>
       <c r="I133">
@@ -44645,7 +44645,7 @@
         <v>0</v>
       </c>
       <c r="H134" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A134,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H134),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A134,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H134),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A134,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H134),2))</f>
         <v>14.16</v>
       </c>
       <c r="I134">
@@ -44698,7 +44698,7 @@
         <v>0</v>
       </c>
       <c r="H135" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A135,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H135),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A135,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H135),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A135,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H135),2))</f>
         <v>4.3899999999999997</v>
       </c>
       <c r="I135">
@@ -44751,7 +44751,7 @@
         <v>0</v>
       </c>
       <c r="H136" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A136,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H136),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A136,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H136),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A136,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H136),2))</f>
         <v>8.7899999999999991</v>
       </c>
       <c r="I136">
@@ -44804,7 +44804,7 @@
         <v>0</v>
       </c>
       <c r="H137" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A137,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H137),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A137,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H137),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A137,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H137),2))</f>
         <v>14.16</v>
       </c>
       <c r="I137">
@@ -44857,7 +44857,7 @@
         <v>0</v>
       </c>
       <c r="H138" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A138,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H138),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A138,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H138),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A138,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H138),2))</f>
         <v>4.3899999999999997</v>
       </c>
       <c r="I138">
@@ -44910,7 +44910,7 @@
         <v>0</v>
       </c>
       <c r="H139" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A139,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H139),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A139,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H139),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A139,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H139),2))</f>
         <v>8.7899999999999991</v>
       </c>
       <c r="I139">
@@ -44963,7 +44963,7 @@
         <v>0</v>
       </c>
       <c r="H140" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A140,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H140),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A140,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H140),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A140,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H140),2))</f>
         <v>14.16</v>
       </c>
       <c r="I140">
@@ -45016,7 +45016,7 @@
         <v>0</v>
       </c>
       <c r="H141" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A141,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H141),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A141,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H141),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A141,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H141),2))</f>
         <v>2.06</v>
       </c>
       <c r="I141">
@@ -45069,7 +45069,7 @@
         <v>0</v>
       </c>
       <c r="H142" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A142,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H142),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A142,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H142),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A142,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H142),2))</f>
         <v>3.07</v>
       </c>
       <c r="I142">
@@ -45122,7 +45122,7 @@
         <v>0</v>
       </c>
       <c r="H143" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A143,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H143),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A143,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H143),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A143,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H143),2))</f>
         <v>4.3</v>
       </c>
       <c r="I143">
@@ -45175,7 +45175,7 @@
         <v>0</v>
       </c>
       <c r="H144" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A144,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H144),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A144,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H144),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A144,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H144),2))</f>
         <v>2.06</v>
       </c>
       <c r="I144">
@@ -45228,7 +45228,7 @@
         <v>0</v>
       </c>
       <c r="H145" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A145,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H145),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A145,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H145),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A145,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H145),2))</f>
         <v>3.07</v>
       </c>
       <c r="I145">
@@ -45281,7 +45281,7 @@
         <v>0</v>
       </c>
       <c r="H146" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A146,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H146),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A146,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H146),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A146,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H146),2))</f>
         <v>4.3</v>
       </c>
       <c r="I146">
@@ -45334,7 +45334,7 @@
         <v>0</v>
       </c>
       <c r="H147" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A147,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H147),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A147,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H147),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A147,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H147),2))</f>
         <v>2.06</v>
       </c>
       <c r="I147">
@@ -45387,7 +45387,7 @@
         <v>0</v>
       </c>
       <c r="H148" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A148,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H148),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A148,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H148),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A148,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H148),2))</f>
         <v>3.07</v>
       </c>
       <c r="I148">
@@ -45440,7 +45440,7 @@
         <v>0</v>
       </c>
       <c r="H149" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A149,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H149),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A149,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H149),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A149,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H149),2))</f>
         <v>4.3</v>
       </c>
       <c r="I149">
@@ -45493,7 +45493,7 @@
         <v>0</v>
       </c>
       <c r="H150" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A150,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H150),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A150,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H150),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A150,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H150),2))</f>
         <v>2.06</v>
       </c>
       <c r="I150">
@@ -45546,7 +45546,7 @@
         <v>0</v>
       </c>
       <c r="H151" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A151,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H151),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A151,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H151),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A151,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H151),2))</f>
         <v>3.07</v>
       </c>
       <c r="I151">
@@ -45599,7 +45599,7 @@
         <v>0</v>
       </c>
       <c r="H152" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A152,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H152),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A152,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H152),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A152,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H152),2))</f>
         <v>4.3</v>
       </c>
       <c r="I152">
@@ -45666,7 +45666,7 @@
         <v>0</v>
       </c>
       <c r="H154" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A154,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H154),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A154,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H154),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A154,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H154),2))</f>
         <v>-1.1599999999999999</v>
       </c>
       <c r="I154">
@@ -45719,8 +45719,8 @@
         <v>0</v>
       </c>
       <c r="H155" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A155,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H155),2)</f>
-        <v>-5.61</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A155,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H155),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A155,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H155),2))</f>
+        <v>-4</v>
       </c>
       <c r="I155">
         <v>2</v>
@@ -45772,8 +45772,8 @@
         <v>0</v>
       </c>
       <c r="H156" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A156,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H156),2)</f>
-        <v>-8.24</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A156,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H156),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A156,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H156),2))</f>
+        <v>-4</v>
       </c>
       <c r="I156">
         <v>2</v>
@@ -45825,8 +45825,8 @@
         <v>0</v>
       </c>
       <c r="H157" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A157,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H157),2)</f>
-        <v>-10.63</v>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A157,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H157),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A157,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H157),2))</f>
+        <v>-4</v>
       </c>
       <c r="I157">
         <v>2</v>
@@ -45879,7 +45879,7 @@
         <v>0</v>
       </c>
       <c r="H158" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A158,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H158),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A158,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H158),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A158,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H158),2))</f>
         <v>0.01</v>
       </c>
       <c r="I158">
@@ -45932,7 +45932,7 @@
         <v>0</v>
       </c>
       <c r="H159" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A159,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H159),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A159,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H159),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A159,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H159),2))</f>
         <v>0.01</v>
       </c>
       <c r="I159">
@@ -45985,7 +45985,7 @@
         <v>0</v>
       </c>
       <c r="H160" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A160,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H160),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A160,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H160),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A160,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H160),2))</f>
         <v>2.06</v>
       </c>
       <c r="I160">
@@ -46038,7 +46038,7 @@
         <v>0</v>
       </c>
       <c r="H161" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A161,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H161),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A161,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H161),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A161,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H161),2))</f>
         <v>3.07</v>
       </c>
       <c r="I161">
@@ -46105,7 +46105,7 @@
         <v>0</v>
       </c>
       <c r="H163" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A163,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H163),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A163,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H163),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A163,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H163),2))</f>
         <v>0.78</v>
       </c>
       <c r="I163">
@@ -46158,7 +46158,7 @@
         <v>0</v>
       </c>
       <c r="H164" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A164,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H164),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A164,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H164),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A164,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H164),2))</f>
         <v>0.45</v>
       </c>
       <c r="I164">
@@ -46211,7 +46211,7 @@
         <v>0</v>
       </c>
       <c r="H165" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A165,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H165),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A165,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H165),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A165,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H165),2))</f>
         <v>0.1</v>
       </c>
       <c r="I165">
@@ -46278,7 +46278,7 @@
         <v>1</v>
       </c>
       <c r="H167" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A167,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H167),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A167,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H167),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A167,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H167),2))</f>
         <v>-0.6</v>
       </c>
       <c r="I167">
@@ -46331,7 +46331,7 @@
         <v>1</v>
       </c>
       <c r="H168" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A168,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H168),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A168,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H168),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A168,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H168),2))</f>
         <v>-0.81</v>
       </c>
       <c r="I168">
@@ -46384,7 +46384,7 @@
         <v>1</v>
       </c>
       <c r="H169" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A169,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H169),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A169,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H169),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A169,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H169),2))</f>
         <v>-1.01</v>
       </c>
       <c r="I169">
@@ -46437,7 +46437,7 @@
         <v>1</v>
       </c>
       <c r="H170" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A170,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H170),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A170,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H170),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A170,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H170),2))</f>
         <v>-1.01</v>
       </c>
       <c r="I170">
@@ -46490,7 +46490,7 @@
         <v>0</v>
       </c>
       <c r="H171" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A171,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H171),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A171,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H171),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A171,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H171),2))</f>
         <v>5.88</v>
       </c>
       <c r="I171">
@@ -46543,7 +46543,7 @@
         <v>0</v>
       </c>
       <c r="H172" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A172,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H172),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A172,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H172),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A172,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H172),2))</f>
         <v>8.7100000000000009</v>
       </c>
       <c r="I172">
@@ -46610,7 +46610,7 @@
         <v>0</v>
       </c>
       <c r="H174" s="5">
-        <f ca="1">ROUND(_xlfn.IFNA(VLOOKUP(A174,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H174),2)</f>
+        <f ca="1">IF(ROUND(_xlfn.IFNA(VLOOKUP(A174,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H174),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A174,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H174),2))</f>
         <v>3.13</v>
       </c>
       <c r="I174">
@@ -46676,7 +46676,7 @@
         <v>0</v>
       </c>
       <c r="H176" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A176,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H176),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A176,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H176),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A176,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H176),2))</f>
         <v>0</v>
       </c>
       <c r="I176">
@@ -46728,7 +46728,7 @@
         <v>0</v>
       </c>
       <c r="H177" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A177,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H177),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A177,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H177),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A177,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H177),2))</f>
         <v>0</v>
       </c>
       <c r="I177">
@@ -46780,7 +46780,7 @@
         <v>0</v>
       </c>
       <c r="H178" s="5">
-        <f>ROUND(_xlfn.IFNA(VLOOKUP(A178,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H178),2)</f>
+        <f>IF(ROUND(_xlfn.IFNA(VLOOKUP(A178,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H178),2)&lt;-4,-4,ROUND(_xlfn.IFNA(VLOOKUP(A178,'Weapon Formulas'!$E$10:$L$300,7,0),weapon_components!H178),2))</f>
         <v>0</v>
       </c>
       <c r="I178">

</xml_diff>

<commit_message>
HardAI cruiser section templates complete
</commit_message>
<xml_diff>
--- a/Stellaris Rebalance.xlsx
+++ b/Stellaris Rebalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="737" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="737" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weapon_components" sheetId="4" r:id="rId1"/>
@@ -20168,8 +20168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP178"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S113" sqref="S113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20880,7 +20880,7 @@
         <v>1.8277475516866157</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" ref="H12:H25" si="14">$F13*(INDEX($F$3:$F$5,H$9)+(($C13+($D13*$F$7))*INDEX($G$3:$G$5,H$9)))</f>
+        <f t="shared" ref="H13:H25" si="14">$F13*(INDEX($F$3:$F$5,H$9)+(($C13+($D13*$F$7))*INDEX($G$3:$G$5,H$9)))</f>
         <v>1.6797</v>
       </c>
       <c r="I13" s="2">
@@ -31506,7 +31506,7 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="R141" s="38">
-        <f t="shared" ref="R141:R175" si="99">IF((F141*INDEX($O$2:$O$6,$C141))/((F141-H141)+0.001)&gt;1,1,IF((F141*INDEX($O$2:$O$6,$C141))/((F141-H141)+0.001)&lt;0,1,(F141*INDEX($O$2:$O$6,$C141))/((F141-H141)+0.001)))</f>
+        <f t="shared" ref="R141:R173" si="99">IF((F141*INDEX($O$2:$O$6,$C141))/((F141-H141)+0.001)&gt;1,1,IF((F141*INDEX($O$2:$O$6,$C141))/((F141-H141)+0.001)&lt;0,1,(F141*INDEX($O$2:$O$6,$C141))/((F141-H141)+0.001)))</f>
         <v>0.39950678175092486</v>
       </c>
       <c r="S141" s="32">
@@ -34354,7 +34354,7 @@
         <v>0.6</v>
       </c>
       <c r="D9" s="12">
-        <f t="shared" ref="C9:E9" si="6">(VLOOKUP(D10,$E$28:$F$102,2,1)/100)</f>
+        <f t="shared" ref="D9:E9" si="6">(VLOOKUP(D10,$E$28:$F$102,2,1)/100)</f>
         <v>0.4</v>
       </c>
       <c r="E9" s="12">
@@ -38279,8 +38279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M5" sqref="A1:O178"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>